<commit_message>
Move MalwareAttribution proj one folder down
</commit_message>
<xml_diff>
--- a/data/test_data.xlsx
+++ b/data/test_data.xlsx
@@ -31,6 +31,21 @@
     <t>network_udp_dst</t>
   </si>
   <si>
+    <t>playtech</t>
+  </si>
+  <si>
+    <t>022c025365bc4875a116877a3d2648a6</t>
+  </si>
+  <si>
+    <t>SetErrorMode OleInitialize LdrGetDllHandle LdrGetDllHandle LdrLoadDll LdrGetProcedureAddress LdrLoadDll LdrGetProcedureAddress LdrLoadDll LdrGetProcedureAddress LdrGetProcedureAddress NtOpenSection NtMapViewOfSection RegOpenKeyExW RegQueryValueExW RegCloseKey RegOpenKeyExW RegOpenKeyExW RegQueryValueExW RegCloseKey RegOpenKeyExW RegOpenKeyExW RegQueryValueExW RegCloseKey RegOpenKeyExW RegOpenKeyExW RegQueryValueExW RegCloseKey RegOpenKeyExW RegOpenKeyExW RegQueryValueExW RegCloseKey RegOpenKeyExW NtClose NtOpenKey NtQueryValueKey NtClose NtOpenKey NtQueryValueKey NtClose LdrLoadDll LdrGetProcedureAddress LdrGetProcedureAddress GetSystemWindowsDirectoryW NtCreateFile NtCreateSection NtMapViewOfSection NtClose NtClose RegOpenKeyExA LdrGetProcedureAddress CreateActCtxW LdrLoadDll LdrLoadDll LdrGetProcedureAddress GetSystemDirectoryW RegOpenKeyExA RegOpenKeyExA LdrLoadDll LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress RegOpenKeyExW RegQueryValueExW RegCloseKey RegOpenKeyExW LdrGetProcedureAddress LdrGetProcedureAddress RegOpenKeyExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegCloseKey LdrGetProcedureAddress RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegQueryValueExW RegCloseKey LdrGetProcedureAddress LdrGetProcedureAddress GetVolumeNameForVolumeMountPointW LdrGetProcedureAddress RegOpenKeyExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegCloseKey RegOpenKeyExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegCloseKey LdrGetProcedureAddress NtClose RegOpenKeyExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegCloseKey RegOpenKeyExW LdrLoadDll LdrGetProcedureAddress RegEnumKeyW RegOpenKeyExW RegQueryValueExW RegCloseKey RegEnumKeyW RegCloseKey LdrGetProcedureAddress RegOpenKeyExW RegOpenKeyExW NtCreateFile NtClose NtQueryDirectoryFile NtClose LdrGetProcedureAddress CoCreateInstance NtOpenSection NtOpenSection CreateDirectoryW NtCreateFile GetSystemWindowsDirectoryW GetSystemWindowsDirectoryW GetSystemWindowsDirectoryW LoadStringW GetSystemWindowsDirectoryW GetSystemDirectoryW RegOpenKeyExW LdrLoadDll LdrGetProcedureAddress RegQueryValueExW RegCloseKey RegOpenKeyExW RegQueryValueExW RegCloseKey NtCreateMutant NtCreateMutant GetNativeSystemInfo GetSystemWindowsDirectoryW GetSystemWindowsDirectoryW NtClose LdrLoadDll LdrGetProcedureAddress LdrLoadDll NtQuerySystemInformation RegOpenKeyExA RegQueryValueExA RegCloseKey NtOpenKey NtQueryValueKey NtClose NtOpenKey NtQueryValueKey NtClose NtOpenKey NtQueryValueKey NtClose RegOpenKeyExW GlobalMemoryStatusEx NtOpenKey NtOpenKey NtQueryValueKey NtClose NtDuplicateObject LdrGetProcedureAddress NtDuplicateObject NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory GetVolumeNameForVolumeMountPointW NtClose RegOpenKeyExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegCloseKey RegOpenKeyExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegCloseKey NtClose LdrGetProcedureAddress LdrGetProcedureAddress RegOpenKeyExW RegQueryValueExW RegQueryValueExW GetSystemTimeAsFileTime GetSystemTimeAsFileTime RegOpenKeyExW RegQueryValueExW RegCloseKey RegOpenKeyExW RegQueryValueExW RegCloseKey RegOpenKeyExW RegQueryValueExW RegCloseKey LdrLoadDll LdrGetProcedureAddress RegCloseKey NtClose LdrGetProcedureAddress NtCreateSection NtClose NtMapViewOfSection NtOpenSection NtCreateFile NtClose NtCreateSection NtClose NtMapViewOfSection NtDuplicateObject GetVolumeNameForVolumeMountPointW NtClose RegOpenKeyExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegCloseKey RegOpenKeyExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegCloseKey NtDuplicateObject NtClose GetVolumeNameForVolumeMountPointW NtClose RegOpenKeyExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegCloseKey RegOpenKeyExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegCloseKey LdrGetProcedureAddress GetVolumePathNamesForVolumeNameW GetVolumePathNamesForVolumeNameW NtClose GetVolumePathNamesForVolumeNameW GetVolumePathNamesForVolumeNameW NtClose GetVolumePathNamesForVolumeNameW GetVolumePathNamesForVolumeNameW GetVolumePathNamesForVolumeNameW GetVolumePathNamesForVolumeNameW NtClose LdrGetProcedureAddress LdrUnloadDll NtClose LdrGetProcedureAddress LdrGetProcedureAddress GetSystemTimeAsFileTime NtOpenSection NtMapViewOfSection GetSystemTimeAsFileTime GetSystemTimeAsFileTime GetSystemTimeAsFileTime NtClose NtClose NtUnmapViewOfSection NtCreateFile GetFileSizeEx NtReadFile GetFileInformationByHandleEx NtClose GetSystemTimeAsFileTime LdrGetProcedureAddress GetSystemTimeAsFileTime RegOpenKeyExW RegQueryValueExW RegCloseKey RegOpenKeyExW LdrLoadDll LdrGetProcedureAddress RegOpenKeyExW RegOpenKeyExW RegQueryValueExW RegQueryValueExW RegCloseKey RegOpenKeyExW RegQueryValueExW RegCloseKey RegOpenKeyExW RegOpenKeyExW RegQueryValueExW RegCloseKey RegOpenKeyExW RegOpenKeyExW RegQueryValueExW RegCloseKey RegOpenKeyExW RegOpenKeyExW RegQueryValueExW RegCloseKey RegOpenKeyExW RegOpenKeyExW RegQueryValueExW RegCloseKey RegOpenKeyExW RegOpenKeyExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegCloseKey LdrLoadDll LdrGetProcedureAddress RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegCloseKey RegOpenKeyExW RegCloseKey RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegQueryValueExW RegOpenKeyExW RegQueryValueExW RegOpenKeyExW RegQueryValueExW RegOpenKeyExW RegQueryValueExW RegOpenKeyExW RegQueryValueExW RegOpenKeyExW RegQueryValueExW RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegCloseKey RegCloseKey RegCloseKey NtCreateFile NtClose NtQueryDirectoryFile NtClose GetSystemTimeAsFileTime NtCreateFile NtClose NtQueryDirectoryFile NtClose NtCreateFile NtClose NtQueryDirectoryFile NtClose NtCreateFile NtClose NtQueryDirectoryFile NtClose RegOpenKeyExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegOpenKeyExW RegCloseKey LdrGetProcedureAddress CoInitializeEx NtOpenProcess NtClose RegOpenKeyExW RegOpenKeyExW RegCloseKey NtClose NtOpenKey RegOpenKeyExW RegCloseKey RegQueryValueExW RegCloseKey GetSystemTimeAsFileTime GetFileAttributesExW NtOpenFile NtQueryInformationFile NtAllocateVirtualMemory NtAllocateVirtualMemory NtReadFile NtFreeVirtualMemory NtClose NtOpenFile NtQueryInformationFile NtAllocateVirtualMemory NtAllocateVirtualMemory NtReadFile NtFreeVirtualMemory NtClose NtOpenFile NtQueryInformationFile NtAllocateVirtualMemory NtAllocateVirtualMemory NtReadFile NtFreeVirtualMemory NtClose LdrGetProcedureAddress CoUninitialize RegOpenKeyExW RegOpenKeyExW GetSystemTimeAsFileTime RegOpenKeyExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegOpenKeyExW RegCloseKey CoInitializeEx NtOpenProcess NtClose RegOpenKeyExW RegOpenKeyExW RegCloseKey NtClose NtOpenKey RegOpenKeyExW RegCloseKey RegQueryValueExW RegOpenKeyExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegOpenKeyExW RegCloseKey NtOpenProcess NtClose RegOpenKeyExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegCloseKey CoUninitialize GetSystemTimeAsFileTime RegOpenKeyExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegOpenKeyExW RegCloseKey CoInitializeEx LdrLoadDll LdrGetProcedureAddress LdrLoadDll LdrGetProcedureAddress RegOpenKeyExW RegQueryValueExW RegQueryValueExW RegCloseKey NtClose CoUninitialize GetSystemTimeAsFileTime RegOpenKeyExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegOpenKeyExW RegCloseKey CoInitializeEx CoUninitialize GetSystemTimeAsFileTime RegOpenKeyExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegCloseKey RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegQueryValueExW RegCloseKey LdrGetDllHandle LdrGetDllHandle LdrGetProcedureAddress LdrGetProcedureAddress RegOpenKeyExW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegCloseKey RegOpenKeyExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegOpenKeyExW RegCloseKey NtOpenProcess NtClose RegOpenKeyExW RegOpenKeyExW RegCloseKey NtClose NtOpenKey RegOpenKeyExW RegCloseKey RegQueryValueExW RegOpenKeyExW RegQueryValueExW RegQueryValueExW RegCloseKey NtClose RegCloseKey RegOpenKeyExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegOpenKeyExW RegCloseKey RegOpenKeyExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegOpenKeyExW RegCloseKey RegOpenKeyExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegOpenKeyExW RegCloseKey RegOpenKeyExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegOpenKeyExW RegCloseKey RegOpenKeyExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegOpenKeyExW RegCloseKey RegOpenKeyExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegOpenKeyExW RegCloseKey RegOpenKeyExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegOpenKeyExW RegCloseKey RegOpenKeyExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegOpenKeyExW RegCloseKey RegOpenKeyExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegOpenKeyExW RegCloseKey RegOpenKeyExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegOpenKeyExW RegCloseKey NtOpenProcess NtClose RegOpenKeyExW RegOpenKeyExW RegCloseKey NtClose NtOpenKey RegOpenKeyExW RegCloseKey RegQueryValueExW RegCloseKey RegOpenKeyExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegOpenKeyExW RegCloseKey RegOpenKeyExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegOpenKeyExW RegCloseKey RegOpenKeyExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegOpenKeyExW RegCloseKey RegOpenKeyExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegOpenKeyExW RegCloseKey RegOpenKeyExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegOpenKeyExW RegCloseKey RegOpenKeyExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegOpenKeyExW RegCloseKey RegOpenKeyExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegOpenKeyExW RegCloseKey NtFreeVirtualMemory NtFreeVirtualMemory NtOpenProcess NtClose RegOpenKeyExW RegOpenKeyExW RegCloseKey NtClose NtAllocateVirtualMemory NtOpenKey RegOpenKeyExW RegCloseKey RegQueryValueExW RegCloseKey RegOpenKeyExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegOpenKeyExW RegCloseKey RegOpenKeyExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegOpenKeyExW RegCloseKey RegOpenKeyExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegOpenKeyExW RegCloseKey RegOpenKeyExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegOpenKeyExW RegCloseKey RegOpenKeyExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegOpenKeyExW RegCloseKey RegOpenKeyExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegOpenKeyExW RegCloseKey RegOpenKeyExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegOpenKeyExW RegCloseKey RegOpenKeyExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegOpenKeyExW RegCloseKey RegOpenKeyExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegOpenKeyExW RegCloseKey RegOpenKeyExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegOpenKeyExW RegCloseKey RegOpenKeyExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegOpenKeyExW RegCloseKey RegOpenKeyExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegOpenKeyExW RegCloseKey RegOpenKeyExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegOpenKeyExW RegCloseKey RegOpenKeyExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegOpenKeyExW RegCloseKey RegOpenKeyExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegOpenKeyExW RegCloseKey NtOpenProcess NtClose RegOpenKeyExW RegOpenKeyExW RegCloseKey NtClose NtOpenKey RegOpenKeyExW RegCloseKey RegQueryValueExW RegOpenKeyExW RegQueryValueExW RegQueryValueExW RegCloseKey NtClose RegCloseKey RegOpenKeyExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegOpenKeyExW RegCloseKey RegOpenKeyExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegOpenKeyExW RegCloseKey RegOpenKeyExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegOpenKeyExW RegCloseKey RegOpenKeyExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegOpenKeyExW RegCloseKey RegOpenKeyExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegOpenKeyExW RegCloseKey RegOpenKeyExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegOpenKeyExW RegCloseKey RegOpenKeyExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegOpenKeyExW RegCloseKey RegOpenKeyExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegOpenKeyExW RegCloseKey NtOpenProcess NtClose RegOpenKeyExW RegOpenKeyExW RegCloseKey NtClose NtOpenKey RegOpenKeyExW RegCloseKey RegQueryValueExW RegCloseKey RegOpenKeyExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegOpenKeyExW RegCloseKey RegOpenKeyExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegOpenKeyExW RegCloseKey RegOpenKeyExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegOpenKeyExW RegCloseKey RegOpenKeyExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegOpenKeyExW RegCloseKey RegOpenKeyExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegOpenKeyExW RegCloseKey RegOpenKeyExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegOpenKeyExW RegCloseKey NtOpenProcess NtClose RegOpenKeyExW RegOpenKeyExW RegCloseKey NtClose NtOpenKey RegOpenKeyExW RegCloseKey RegQueryValueExW RegCloseKey RegOpenKeyExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegOpenKeyExW RegCloseKey RegOpenKeyExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegOpenKeyExW RegCloseKey RegOpenKeyExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegOpenKeyExW RegCloseKey RegOpenKeyExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQue</t>
+  </si>
+  <si>
+    <t>192.168.56.101:49360 192.168.56.101:64412 192.168.56.101:50300 192.168.56.101:137 192.168.56.101:1900 192.168.56.101:49362 192.168.56.101:58084 192.168.56.101:54425 192.168.56.101:138 192.168.56.101:54426 192.168.56.101:54428 192.168.56.101:54430 192.168.56.101:52057 192.168.56.101:59469 192.168.56.101:54227 192.168.56.101:54228 192.168.56.101:52887 192.168.56.101:63529 192.168.56.101:51765 192.168.56.101:49465 192.168.56.101:50974 192.168.56.101:55167 192.168.56.101:63794 192.168.56.101:62948 192.168.56.101:49746 192.168.56.101:53485 192.168.56.101:54813 192.168.56.101:63393 192.168.56.101:61926 192.168.56.101:55972 192.168.56.101:50766 192.168.56.101:51753 192.168.56.101:50018 192.168.56.101:50988 192.168.56.101:62982 192.168.56.101:56409 192.168.56.101:60009 192.168.56.101:50639 192.168.56.101:53003 192.168.56.101:58359 192.168.56.101:61815 192.168.56.101:64235 192.168.56.101:52402 192.168.56.101:62413 192.168.56.101:59538</t>
+  </si>
+  <si>
+    <t>8.8.8.8:53 224.0.0.252:5355 239.255.255.250:3702 192.168.56.255:137 239.255.255.250:1900 239.255.255.250:1900 224.0.0.252:5355 8.8.8.8:53 192.168.56.255:138 239.255.255.250:3702 239.255.255.250:3702 239.255.255.250:3702 224.0.0.252:5355 224.0.0.252:5355 224.0.0.252:5355 239.255.255.250:3702 224.0.0.252:5355 224.0.0.252:5355 224.0.0.252:5355 224.0.0.252:5355 8.8.8.8:53 8.8.8.8:53 224.0.0.252:5355 224.0.0.252:5355 224.0.0.252:5355 224.0.0.252:5355 8.8.8.8:53 8.8.8.8:53 224.0.0.252:5355 224.0.0.252:5355 224.0.0.252:5355 224.0.0.252:5355 8.8.8.8:53 8.8.8.8:53 224.0.0.252:5355 224.0.0.252:5355 224.0.0.252:5355 224.0.0.252:5355 224.0.0.252:5355 224.0.0.252:5355 8.8.8.8:53 8.8.8.8:53 8.8.8.8:53 8.8.8.8:53 8.8.8.8:53</t>
+  </si>
+  <si>
     <t>onlinegames</t>
   </si>
   <si>
@@ -44,21 +59,6 @@
   </si>
   <si>
     <t>224.0.0.252:5355 8.8.8.8:53 239.255.255.250:3702 192.168.56.255:137 239.255.255.250:1900 239.255.255.250:1900 224.0.0.252:5355 239.255.255.250:3702 8.8.8.8:53 192.168.56.255:138 224.0.0.252:5355 224.0.0.252:5355 224.0.0.252:5355 239.255.255.250:3702 224.0.0.252:5355 8.8.8.8:53 224.0.0.252:5355 224.0.0.252:5355 224.0.0.252:5355 8.8.8.8:53</t>
-  </si>
-  <si>
-    <t>playtech</t>
-  </si>
-  <si>
-    <t>03ad0aea1dc1f1fd3d9c441a063f23e6</t>
-  </si>
-  <si>
-    <t>SetErrorMode OleInitialize LdrGetDllHandle LdrGetDllHandle LdrLoadDll LdrGetProcedureAddress LdrLoadDll LdrGetProcedureAddress LdrLoadDll LdrGetProcedureAddress LdrGetProcedureAddress NtOpenSection NtMapViewOfSection RegOpenKeyExW RegQueryValueExW RegCloseKey RegOpenKeyExW RegOpenKeyExW RegQueryValueExW RegCloseKey RegOpenKeyExW RegOpenKeyExW RegQueryValueExW RegCloseKey RegOpenKeyExW RegOpenKeyExW RegQueryValueExW RegCloseKey RegOpenKeyExW RegOpenKeyExW RegQueryValueExW RegCloseKey RegOpenKeyExW NtClose NtOpenKey NtQueryValueKey NtClose NtOpenKey NtQueryValueKey NtClose LdrLoadDll LdrGetProcedureAddress LdrGetProcedureAddress GetSystemWindowsDirectoryW NtCreateFile NtCreateSection NtMapViewOfSection NtClose NtClose RegOpenKeyExA LdrGetProcedureAddress CreateActCtxW LdrLoadDll LdrLoadDll LdrGetProcedureAddress GetSystemDirectoryW RegOpenKeyExA RegOpenKeyExA LdrLoadDll LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress RegOpenKeyExW RegQueryValueExW RegCloseKey RegOpenKeyExW LdrGetProcedureAddress LdrGetProcedureAddress RegOpenKeyExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegCloseKey LdrGetProcedureAddress RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegQueryValueExW RegCloseKey LdrGetProcedureAddress LdrGetProcedureAddress GetVolumeNameForVolumeMountPointW LdrGetProcedureAddress RegOpenKeyExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegCloseKey RegOpenKeyExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegCloseKey LdrGetProcedureAddress NtClose RegOpenKeyExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegCloseKey RegOpenKeyExW LdrLoadDll LdrGetProcedureAddress RegEnumKeyW RegOpenKeyExW RegQueryValueExW RegCloseKey RegEnumKeyW RegCloseKey LdrGetProcedureAddress RegOpenKeyExW RegOpenKeyExW NtCreateFile NtClose NtQueryDirectoryFile NtClose LdrGetProcedureAddress CoCreateInstance NtOpenSection NtOpenSection CreateDirectoryW NtCreateFile GetSystemWindowsDirectoryW GetSystemWindowsDirectoryW GetSystemWindowsDirectoryW LoadStringW GetSystemWindowsDirectoryW GetSystemDirectoryW RegOpenKeyExW LdrLoadDll LdrGetProcedureAddress RegQueryValueExW RegCloseKey RegOpenKeyExW RegQueryValueExW RegCloseKey NtCreateMutant NtCreateMutant GetNativeSystemInfo GetSystemWindowsDirectoryW GetSystemWindowsDirectoryW NtClose LdrLoadDll LdrGetProcedureAddress LdrLoadDll NtQuerySystemInformation RegOpenKeyExA RegQueryValueExA RegCloseKey NtOpenKey NtQueryValueKey NtClose NtOpenKey NtQueryValueKey NtClose NtOpenKey NtQueryValueKey NtClose RegOpenKeyExW GlobalMemoryStatusEx NtOpenKey NtOpenKey NtQueryValueKey NtClose NtDuplicateObject NtAllocateVirtualMemory NtAllocateVirtualMemory LdrGetProcedureAddress NtDuplicateObject NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory GetVolumeNameForVolumeMountPointW NtClose NtAllocateVirtualMemory RegOpenKeyExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegCloseKey RegOpenKeyExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegCloseKey NtClose LdrGetProcedureAddress LdrGetProcedureAddress RegOpenKeyExW RegQueryValueExW RegQueryValueExW GetSystemTimeAsFileTime GetSystemTimeAsFileTime RegOpenKeyExW RegQueryValueExW RegCloseKey RegOpenKeyExW RegQueryValueExW RegCloseKey RegOpenKeyExW RegQueryValueExW RegCloseKey LdrLoadDll LdrGetProcedureAddress RegCloseKey NtClose LdrGetProcedureAddress NtCreateSection NtClose NtMapViewOfSection NtDuplicateObject GetVolumeNameForVolumeMountPointW NtClose RegOpenKeyExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegCloseKey RegOpenKeyExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegCloseKey NtDuplicateObject NtClose GetVolumeNameForVolumeMountPointW NtClose RegOpenKeyExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegCloseKey RegOpenKeyExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegCloseKey LdrGetProcedureAddress GetVolumePathNamesForVolumeNameW GetVolumePathNamesForVolumeNameW NtClose GetVolumePathNamesForVolumeNameW GetVolumePathNamesForVolumeNameW NtClose GetVolumePathNamesForVolumeNameW GetVolumePathNamesForVolumeNameW GetVolumePathNamesForVolumeNameW GetVolumePathNamesForVolumeNameW NtClose LdrGetProcedureAddress LdrUnloadDll NtClose NtOpenSection NtCreateFile NtClose NtCreateSection NtClose NtMapViewOfSection LdrGetProcedureAddress LdrGetProcedureAddress GetSystemTimeAsFileTime NtOpenSection NtMapViewOfSection GetSystemTimeAsFileTime GetSystemTimeAsFileTime GetSystemTimeAsFileTime NtClose NtClose NtUnmapViewOfSection NtCreateFile GetFileSizeEx NtReadFile GetFileInformationByHandleEx NtClose GetSystemTimeAsFileTime LdrGetProcedureAddress GetSystemTimeAsFileTime RegOpenKeyExW RegQueryValueExW RegCloseKey RegOpenKeyExW LdrLoadDll LdrGetProcedureAddress RegOpenKeyExW RegOpenKeyExW RegQueryValueExW RegQueryValueExW RegCloseKey RegOpenKeyExW RegQueryValueExW RegCloseKey RegOpenKeyExW RegOpenKeyExW RegQueryValueExW RegCloseKey RegOpenKeyExW RegOpenKeyExW RegQueryValueExW RegCloseKey RegOpenKeyExW RegOpenKeyExW RegQueryValueExW RegCloseKey RegOpenKeyExW RegOpenKeyExW RegQueryValueExW RegCloseKey RegOpenKeyExW RegOpenKeyExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegCloseKey LdrLoadDll LdrGetProcedureAddress RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegCloseKey RegOpenKeyExW RegCloseKey RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegQueryValueExW RegOpenKeyExW RegQueryValueExW RegOpenKeyExW RegQueryValueExW RegOpenKeyExW RegQueryValueExW RegOpenKeyExW RegQueryValueExW RegOpenKeyExW RegQueryValueExW RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegCloseKey RegCloseKey RegCloseKey NtCreateFile NtClose NtQueryDirectoryFile NtClose GetSystemTimeAsFileTime NtAllocateVirtualMemory NtCreateFile NtClose NtQueryDirectoryFile NtClose NtCreateFile NtClose NtQueryDirectoryFile NtClose NtCreateFile NtClose NtQueryDirectoryFile NtClose RegOpenKeyExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegOpenKeyExW RegCloseKey LdrGetProcedureAddress CoInitializeEx NtOpenProcess NtClose RegOpenKeyExW RegOpenKeyExW RegCloseKey NtClose NtOpenKey RegOpenKeyExW RegCloseKey RegQueryValueExW RegCloseKey GetSystemTimeAsFileTime GetFileAttributesExW NtOpenFile NtQueryInformationFile NtAllocateVirtualMemory NtAllocateVirtualMemory NtReadFile NtFreeVirtualMemory NtClose NtOpenFile NtQueryInformationFile NtAllocateVirtualMemory NtAllocateVirtualMemory NtReadFile NtFreeVirtualMemory NtClose NtOpenFile NtQueryInformationFile NtAllocateVirtualMemory NtAllocateVirtualMemory NtReadFile NtFreeVirtualMemory NtClose LdrGetProcedureAddress CoUninitialize RegOpenKeyExW RegOpenKeyExW GetSystemTimeAsFileTime RegOpenKeyExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegOpenKeyExW RegCloseKey CoInitializeEx NtOpenProcess NtClose RegOpenKeyExW RegOpenKeyExW RegCloseKey NtClose NtOpenKey RegOpenKeyExW RegCloseKey RegQueryValueExW RegOpenKeyExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegOpenKeyExW RegCloseKey NtOpenProcess NtClose RegOpenKeyExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegCloseKey NtAllocateVirtualMemory CoUninitialize GetSystemTimeAsFileTime RegOpenKeyExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegOpenKeyExW RegCloseKey CoInitializeEx LdrLoadDll LdrGetProcedureAddress LdrLoadDll LdrGetProcedureAddress RegOpenKeyExW RegQueryValueExW RegQueryValueExW RegCloseKey NtClose CoUninitialize GetSystemTimeAsFileTime RegOpenKeyExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegOpenKeyExW RegCloseKey CoInitializeEx CoUninitialize GetSystemTimeAsFileTime RegOpenKeyExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegCloseKey RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegQueryValueExW RegCloseKey LdrGetDllHandle LdrGetDllHandle LdrGetProcedureAddress LdrGetProcedureAddress RegOpenKeyExW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW NtAllocateVirtualMemory RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW NtAllocateVirtualMemory RegCloseKey NtAllocateVirtualMemory RegOpenKeyExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegOpenKeyExW RegCloseKey NtOpenProcess NtClose RegOpenKeyExW RegOpenKeyExW RegCloseKey NtClose NtOpenKey RegOpenKeyExW RegCloseKey RegQueryValueExW RegOpenKeyExW RegQueryValueExW RegQueryValueExW RegCloseKey NtClose RegCloseKey RegOpenKeyExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegOpenKeyExW RegCloseKey RegOpenKeyExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegOpenKeyExW RegCloseKey RegOpenKeyExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegOpenKeyExW RegCloseKey RegOpenKeyExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegOpenKeyExW RegCloseKey RegOpenKeyExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegOpenKeyExW RegCloseKey RegOpenKeyExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegOpenKeyExW RegCloseKey RegOpenKeyExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegOpenKeyExW RegCloseKey RegOpenKeyExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegOpenKeyExW RegCloseKey RegOpenKeyExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegOpenKeyExW RegCloseKey RegOpenKeyExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegOpenKeyExW RegCloseKey NtOpenProcess NtClose RegOpenKeyExW RegOpenKeyExW RegCloseKey NtClose NtOpenKey RegOpenKeyExW RegCloseKey RegQueryValueExW RegCloseKey RegOpenKeyExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegOpenKeyExW RegCloseKey RegOpenKeyExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegOpenKeyExW RegCloseKey RegOpenKeyExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegOpenKeyExW RegCloseKey RegOpenKeyExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegOpenKeyExW RegCloseKey RegOpenKeyExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegOpenKeyExW RegCloseKey RegOpenKeyExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegOpenKeyExW RegCloseKey RegOpenKeyExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegOpenKeyExW RegCloseKey NtOpenProcess NtClose RegOpenKeyExW RegOpenKeyExW RegCloseKey NtClose NtOpenKey RegOpenKeyExW RegCloseKey RegQueryValueExW RegCloseKey RegOpenKeyExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegOpenKeyExW RegCloseKey RegOpenKeyExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegOpenKeyExW RegCloseKey RegOpenKeyExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegOpenKeyExW RegCloseKey RegOpenKeyExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegOpenKeyExW RegCloseKey RegOpenKeyExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegOpenKeyExW RegCloseKey RegOpenKeyExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegOpenKeyExW RegCloseKey RegOpenKeyExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegOpenKeyExW RegCloseKey NtAllocateVirtualMemory RegOpenKeyExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegOpenKeyExW RegCloseKey RegOpenKeyExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegOpenKeyExW RegCloseKey RegOpenKeyExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegOpenKeyExW RegCloseKey RegOpenKeyExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegOpenKeyExW RegCloseKey RegOpenKeyExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegOpenKeyExW RegCloseKey RegOpenKeyExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegOpenKeyExW RegCloseKey RegOpenKeyExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegOpenKeyExW RegCloseKey RegOpenKeyExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegOpenKeyExW RegCloseKey NtOpenProcess NtClose RegOpenKeyExW RegOpenKeyExW RegCloseKey NtClose NtOpenKey RegOpenKeyExW RegCloseKey RegQueryValueExW RegOpenKeyExW RegQueryValueExW RegQueryValueExW RegCloseKey NtClose RegCloseKey RegOpenKeyExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegOpenKeyExW RegCloseKey RegOpenKeyExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegOpenKeyExW RegCloseKey RegOpenKeyExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegOpenKeyExW RegCloseKey RegOpenKeyExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegOpenKeyExW RegCloseKey RegOpenKeyExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegOpenKeyExW RegCloseKey RegOpenKeyExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegOpenKeyExW RegCloseKey RegOpenKeyExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegOpenKeyExW RegCloseKey RegOpenKeyExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegOpenKeyExW RegCloseKey NtAllocateVirtualMemory NtOpenProcess NtClose RegOpenKeyExW RegOpenKeyExW RegCloseKey NtClose NtOpenKey RegOpenKeyExW RegCloseKey RegQueryValueExW RegCloseKey RegOpenKeyExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegOpenKeyExW RegCloseKey RegOpenKeyExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegOpenKeyExW RegCloseKey RegOpenKeyExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegOpenKeyExW RegCloseKey RegOpenKeyExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegOpenKeyExW RegCloseKey RegOpenKeyExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegOpenKeyExW RegCloseKey RegOpenKeyExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegOpenKeyExW RegCloseKey NtAllocateVirtualMemory NtOpenProcess NtClose RegOpenKeyExW RegOpenKeyExW RegCloseKey NtClose NtOpenKey RegOpenKeyExW RegCloseKey RegQueryValueExW RegCloseKey RegOpenKeyExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegOpenKeyExW RegCloseKey RegOpenKeyExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegOpenKeyExW RegCloseKey RegOpenKeyExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegOpenK</t>
-  </si>
-  <si>
-    <t>192.168.56.101:49360 192.168.56.101:64412 192.168.56.101:50300 192.168.56.101:137 192.168.56.101:1900 192.168.56.101:49362 192.168.56.101:64413 192.168.56.101:58084 192.168.56.101:138 192.168.56.101:54425 192.168.56.101:52057 192.168.56.101:52058 192.168.56.101:59469 192.168.56.101:54227 192.168.56.101:54228 192.168.56.101:52887 192.168.56.101:63529 192.168.56.101:51765 192.168.56.101:49465 192.168.56.101:50974 192.168.56.101:55167 192.168.56.101:63794 192.168.56.101:62948 192.168.56.101:49746 192.168.56.101:53485 192.168.56.101:54813 192.168.56.101:63393 192.168.56.101:61926 192.168.56.101:55972 192.168.56.101:50766 192.168.56.101:51753 192.168.56.101:50018 192.168.56.101:50988 192.168.56.101:62982 192.168.56.101:56409 192.168.56.101:60009 192.168.56.101:50639 192.168.56.101:53003 192.168.56.101:58359 192.168.56.101:61815 192.168.56.101:64235 192.168.56.101:52402 192.168.56.101:62413 192.168.56.101:59538</t>
-  </si>
-  <si>
-    <t>8.8.8.8:53 224.0.0.252:5355 239.255.255.250:3702 192.168.56.255:137 239.255.255.250:1900 239.255.255.250:1900 239.255.255.250:3702 224.0.0.252:5355 192.168.56.255:138 224.0.0.252:5355 8.8.8.8:53 239.255.255.250:3702 224.0.0.252:5355 224.0.0.252:5355 239.255.255.250:3702 224.0.0.252:5355 224.0.0.252:5355 224.0.0.252:5355 224.0.0.252:5355 8.8.8.8:53 8.8.8.8:53 224.0.0.252:5355 224.0.0.252:5355 224.0.0.252:5355 224.0.0.252:5355 8.8.8.8:53 8.8.8.8:53 224.0.0.252:5355 224.0.0.252:5355 224.0.0.252:5355 224.0.0.252:5355 8.8.8.8:53 8.8.8.8:53 224.0.0.252:5355 224.0.0.252:5355 224.0.0.252:5355 224.0.0.252:5355 224.0.0.252:5355 224.0.0.252:5355 8.8.8.8:53 8.8.8.8:53 8.8.8.8:53 8.8.8.8:53 8.8.8.8:53</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
Preprocessing.py cleanup and error handling
</commit_message>
<xml_diff>
--- a/data/test_data.xlsx
+++ b/data/test_data.xlsx
@@ -31,34 +31,34 @@
     <t>network_udp_dst</t>
   </si>
   <si>
-    <t>playtech</t>
-  </si>
-  <si>
-    <t>022c025365bc4875a116877a3d2648a6</t>
-  </si>
-  <si>
-    <t>SetErrorMode OleInitialize LdrGetDllHandle LdrGetDllHandle LdrLoadDll LdrGetProcedureAddress LdrLoadDll LdrGetProcedureAddress LdrLoadDll LdrGetProcedureAddress LdrGetProcedureAddress NtOpenSection NtMapViewOfSection RegOpenKeyExW RegQueryValueExW RegCloseKey RegOpenKeyExW RegOpenKeyExW RegQueryValueExW RegCloseKey RegOpenKeyExW RegOpenKeyExW RegQueryValueExW RegCloseKey RegOpenKeyExW RegOpenKeyExW RegQueryValueExW RegCloseKey RegOpenKeyExW RegOpenKeyExW RegQueryValueExW RegCloseKey RegOpenKeyExW NtClose NtOpenKey NtQueryValueKey NtClose NtOpenKey NtQueryValueKey NtClose LdrLoadDll LdrGetProcedureAddress LdrGetProcedureAddress GetSystemWindowsDirectoryW NtCreateFile NtCreateSection NtMapViewOfSection NtClose NtClose RegOpenKeyExA LdrGetProcedureAddress CreateActCtxW LdrLoadDll LdrLoadDll LdrGetProcedureAddress GetSystemDirectoryW RegOpenKeyExA RegOpenKeyExA LdrLoadDll LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress RegOpenKeyExW RegQueryValueExW RegCloseKey RegOpenKeyExW LdrGetProcedureAddress LdrGetProcedureAddress RegOpenKeyExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegCloseKey LdrGetProcedureAddress RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegQueryValueExW RegCloseKey LdrGetProcedureAddress LdrGetProcedureAddress GetVolumeNameForVolumeMountPointW LdrGetProcedureAddress RegOpenKeyExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegCloseKey RegOpenKeyExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegCloseKey LdrGetProcedureAddress NtClose RegOpenKeyExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegCloseKey RegOpenKeyExW LdrLoadDll LdrGetProcedureAddress RegEnumKeyW RegOpenKeyExW RegQueryValueExW RegCloseKey RegEnumKeyW RegCloseKey LdrGetProcedureAddress RegOpenKeyExW RegOpenKeyExW NtCreateFile NtClose NtQueryDirectoryFile NtClose LdrGetProcedureAddress CoCreateInstance NtOpenSection NtOpenSection CreateDirectoryW NtCreateFile GetSystemWindowsDirectoryW GetSystemWindowsDirectoryW GetSystemWindowsDirectoryW LoadStringW GetSystemWindowsDirectoryW GetSystemDirectoryW RegOpenKeyExW LdrLoadDll LdrGetProcedureAddress RegQueryValueExW RegCloseKey RegOpenKeyExW RegQueryValueExW RegCloseKey NtCreateMutant NtCreateMutant GetNativeSystemInfo GetSystemWindowsDirectoryW GetSystemWindowsDirectoryW NtClose LdrLoadDll LdrGetProcedureAddress LdrLoadDll NtQuerySystemInformation RegOpenKeyExA RegQueryValueExA RegCloseKey NtOpenKey NtQueryValueKey NtClose NtOpenKey NtQueryValueKey NtClose NtOpenKey NtQueryValueKey NtClose RegOpenKeyExW GlobalMemoryStatusEx NtOpenKey NtOpenKey NtQueryValueKey NtClose NtDuplicateObject LdrGetProcedureAddress NtDuplicateObject NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory GetVolumeNameForVolumeMountPointW NtClose RegOpenKeyExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegCloseKey RegOpenKeyExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegCloseKey NtClose LdrGetProcedureAddress LdrGetProcedureAddress RegOpenKeyExW RegQueryValueExW RegQueryValueExW GetSystemTimeAsFileTime GetSystemTimeAsFileTime RegOpenKeyExW RegQueryValueExW RegCloseKey RegOpenKeyExW RegQueryValueExW RegCloseKey RegOpenKeyExW RegQueryValueExW RegCloseKey LdrLoadDll LdrGetProcedureAddress RegCloseKey NtClose LdrGetProcedureAddress NtCreateSection NtClose NtMapViewOfSection NtOpenSection NtCreateFile NtClose NtCreateSection NtClose NtMapViewOfSection NtDuplicateObject GetVolumeNameForVolumeMountPointW NtClose RegOpenKeyExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegCloseKey RegOpenKeyExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegCloseKey NtDuplicateObject NtClose GetVolumeNameForVolumeMountPointW NtClose RegOpenKeyExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegCloseKey RegOpenKeyExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegCloseKey LdrGetProcedureAddress GetVolumePathNamesForVolumeNameW GetVolumePathNamesForVolumeNameW NtClose GetVolumePathNamesForVolumeNameW GetVolumePathNamesForVolumeNameW NtClose GetVolumePathNamesForVolumeNameW GetVolumePathNamesForVolumeNameW GetVolumePathNamesForVolumeNameW GetVolumePathNamesForVolumeNameW NtClose LdrGetProcedureAddress LdrUnloadDll NtClose LdrGetProcedureAddress LdrGetProcedureAddress GetSystemTimeAsFileTime NtOpenSection NtMapViewOfSection GetSystemTimeAsFileTime GetSystemTimeAsFileTime GetSystemTimeAsFileTime NtClose NtClose NtUnmapViewOfSection NtCreateFile GetFileSizeEx NtReadFile GetFileInformationByHandleEx NtClose GetSystemTimeAsFileTime LdrGetProcedureAddress GetSystemTimeAsFileTime RegOpenKeyExW RegQueryValueExW RegCloseKey RegOpenKeyExW LdrLoadDll LdrGetProcedureAddress RegOpenKeyExW RegOpenKeyExW RegQueryValueExW RegQueryValueExW RegCloseKey RegOpenKeyExW RegQueryValueExW RegCloseKey RegOpenKeyExW RegOpenKeyExW RegQueryValueExW RegCloseKey RegOpenKeyExW RegOpenKeyExW RegQueryValueExW RegCloseKey RegOpenKeyExW RegOpenKeyExW RegQueryValueExW RegCloseKey RegOpenKeyExW RegOpenKeyExW RegQueryValueExW RegCloseKey RegOpenKeyExW RegOpenKeyExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegCloseKey LdrLoadDll LdrGetProcedureAddress RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegCloseKey RegOpenKeyExW RegCloseKey RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegQueryValueExW RegOpenKeyExW RegQueryValueExW RegOpenKeyExW RegQueryValueExW RegOpenKeyExW RegQueryValueExW RegOpenKeyExW RegQueryValueExW RegOpenKeyExW RegQueryValueExW RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegCloseKey RegCloseKey RegCloseKey NtCreateFile NtClose NtQueryDirectoryFile NtClose GetSystemTimeAsFileTime NtCreateFile NtClose NtQueryDirectoryFile NtClose NtCreateFile NtClose NtQueryDirectoryFile NtClose NtCreateFile NtClose NtQueryDirectoryFile NtClose RegOpenKeyExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegOpenKeyExW RegCloseKey LdrGetProcedureAddress CoInitializeEx NtOpenProcess NtClose RegOpenKeyExW RegOpenKeyExW RegCloseKey NtClose NtOpenKey RegOpenKeyExW RegCloseKey RegQueryValueExW RegCloseKey GetSystemTimeAsFileTime GetFileAttributesExW NtOpenFile NtQueryInformationFile NtAllocateVirtualMemory NtAllocateVirtualMemory NtReadFile NtFreeVirtualMemory NtClose NtOpenFile NtQueryInformationFile NtAllocateVirtualMemory NtAllocateVirtualMemory NtReadFile NtFreeVirtualMemory NtClose NtOpenFile NtQueryInformationFile NtAllocateVirtualMemory NtAllocateVirtualMemory NtReadFile NtFreeVirtualMemory NtClose LdrGetProcedureAddress CoUninitialize RegOpenKeyExW RegOpenKeyExW GetSystemTimeAsFileTime RegOpenKeyExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegOpenKeyExW RegCloseKey CoInitializeEx NtOpenProcess NtClose RegOpenKeyExW RegOpenKeyExW RegCloseKey NtClose NtOpenKey RegOpenKeyExW RegCloseKey RegQueryValueExW RegOpenKeyExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegOpenKeyExW RegCloseKey NtOpenProcess NtClose RegOpenKeyExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegCloseKey CoUninitialize GetSystemTimeAsFileTime RegOpenKeyExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegOpenKeyExW RegCloseKey CoInitializeEx LdrLoadDll LdrGetProcedureAddress LdrLoadDll LdrGetProcedureAddress RegOpenKeyExW RegQueryValueExW RegQueryValueExW RegCloseKey NtClose CoUninitialize GetSystemTimeAsFileTime RegOpenKeyExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegOpenKeyExW RegCloseKey CoInitializeEx CoUninitialize GetSystemTimeAsFileTime RegOpenKeyExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegCloseKey RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegQueryValueExW RegCloseKey LdrGetDllHandle LdrGetDllHandle LdrGetProcedureAddress LdrGetProcedureAddress RegOpenKeyExW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegCloseKey RegOpenKeyExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegOpenKeyExW RegCloseKey NtOpenProcess NtClose RegOpenKeyExW RegOpenKeyExW RegCloseKey NtClose NtOpenKey RegOpenKeyExW RegCloseKey RegQueryValueExW RegOpenKeyExW RegQueryValueExW RegQueryValueExW RegCloseKey NtClose RegCloseKey RegOpenKeyExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegOpenKeyExW RegCloseKey RegOpenKeyExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegOpenKeyExW RegCloseKey RegOpenKeyExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegOpenKeyExW RegCloseKey RegOpenKeyExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegOpenKeyExW RegCloseKey RegOpenKeyExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegOpenKeyExW RegCloseKey RegOpenKeyExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegOpenKeyExW RegCloseKey RegOpenKeyExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegOpenKeyExW RegCloseKey RegOpenKeyExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegOpenKeyExW RegCloseKey RegOpenKeyExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegOpenKeyExW RegCloseKey RegOpenKeyExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegOpenKeyExW RegCloseKey NtOpenProcess NtClose RegOpenKeyExW RegOpenKeyExW RegCloseKey NtClose NtOpenKey RegOpenKeyExW RegCloseKey RegQueryValueExW RegCloseKey RegOpenKeyExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegOpenKeyExW RegCloseKey RegOpenKeyExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegOpenKeyExW RegCloseKey RegOpenKeyExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegOpenKeyExW RegCloseKey RegOpenKeyExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegOpenKeyExW RegCloseKey RegOpenKeyExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegOpenKeyExW RegCloseKey RegOpenKeyExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegOpenKeyExW RegCloseKey RegOpenKeyExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegOpenKeyExW RegCloseKey NtFreeVirtualMemory NtFreeVirtualMemory NtOpenProcess NtClose RegOpenKeyExW RegOpenKeyExW RegCloseKey NtClose NtAllocateVirtualMemory NtOpenKey RegOpenKeyExW RegCloseKey RegQueryValueExW RegCloseKey RegOpenKeyExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegOpenKeyExW RegCloseKey RegOpenKeyExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegOpenKeyExW RegCloseKey RegOpenKeyExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegOpenKeyExW RegCloseKey RegOpenKeyExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegOpenKeyExW RegCloseKey RegOpenKeyExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegOpenKeyExW RegCloseKey RegOpenKeyExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegOpenKeyExW RegCloseKey RegOpenKeyExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegOpenKeyExW RegCloseKey RegOpenKeyExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegOpenKeyExW RegCloseKey RegOpenKeyExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegOpenKeyExW RegCloseKey RegOpenKeyExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegOpenKeyExW RegCloseKey RegOpenKeyExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegOpenKeyExW RegCloseKey RegOpenKeyExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegOpenKeyExW RegCloseKey RegOpenKeyExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegOpenKeyExW RegCloseKey RegOpenKeyExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegOpenKeyExW RegCloseKey RegOpenKeyExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegOpenKeyExW RegCloseKey NtOpenProcess NtClose RegOpenKeyExW RegOpenKeyExW RegCloseKey NtClose NtOpenKey RegOpenKeyExW RegCloseKey RegQueryValueExW RegOpenKeyExW RegQueryValueExW RegQueryValueExW RegCloseKey NtClose RegCloseKey RegOpenKeyExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegOpenKeyExW RegCloseKey RegOpenKeyExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegOpenKeyExW RegCloseKey RegOpenKeyExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegOpenKeyExW RegCloseKey RegOpenKeyExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegOpenKeyExW RegCloseKey RegOpenKeyExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegOpenKeyExW RegCloseKey RegOpenKeyExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegOpenKeyExW RegCloseKey RegOpenKeyExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegOpenKeyExW RegCloseKey RegOpenKeyExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegOpenKeyExW RegCloseKey NtOpenProcess NtClose RegOpenKeyExW RegOpenKeyExW RegCloseKey NtClose NtOpenKey RegOpenKeyExW RegCloseKey RegQueryValueExW RegCloseKey RegOpenKeyExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegOpenKeyExW RegCloseKey RegOpenKeyExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegOpenKeyExW RegCloseKey RegOpenKeyExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegOpenKeyExW RegCloseKey RegOpenKeyExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegOpenKeyExW RegCloseKey RegOpenKeyExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegOpenKeyExW RegCloseKey RegOpenKeyExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegOpenKeyExW RegCloseKey NtOpenProcess NtClose RegOpenKeyExW RegOpenKeyExW RegCloseKey NtClose NtOpenKey RegOpenKeyExW RegCloseKey RegQueryValueExW RegCloseKey RegOpenKeyExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegOpenKeyExW RegCloseKey RegOpenKeyExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegOpenKeyExW RegCloseKey RegOpenKeyExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegOpenKeyExW RegCloseKey RegOpenKeyExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQue</t>
-  </si>
-  <si>
-    <t>192.168.56.101:49360 192.168.56.101:64412 192.168.56.101:50300 192.168.56.101:137 192.168.56.101:1900 192.168.56.101:49362 192.168.56.101:58084 192.168.56.101:54425 192.168.56.101:138 192.168.56.101:54426 192.168.56.101:54428 192.168.56.101:54430 192.168.56.101:52057 192.168.56.101:59469 192.168.56.101:54227 192.168.56.101:54228 192.168.56.101:52887 192.168.56.101:63529 192.168.56.101:51765 192.168.56.101:49465 192.168.56.101:50974 192.168.56.101:55167 192.168.56.101:63794 192.168.56.101:62948 192.168.56.101:49746 192.168.56.101:53485 192.168.56.101:54813 192.168.56.101:63393 192.168.56.101:61926 192.168.56.101:55972 192.168.56.101:50766 192.168.56.101:51753 192.168.56.101:50018 192.168.56.101:50988 192.168.56.101:62982 192.168.56.101:56409 192.168.56.101:60009 192.168.56.101:50639 192.168.56.101:53003 192.168.56.101:58359 192.168.56.101:61815 192.168.56.101:64235 192.168.56.101:52402 192.168.56.101:62413 192.168.56.101:59538</t>
-  </si>
-  <si>
-    <t>8.8.8.8:53 224.0.0.252:5355 239.255.255.250:3702 192.168.56.255:137 239.255.255.250:1900 239.255.255.250:1900 224.0.0.252:5355 8.8.8.8:53 192.168.56.255:138 239.255.255.250:3702 239.255.255.250:3702 239.255.255.250:3702 224.0.0.252:5355 224.0.0.252:5355 224.0.0.252:5355 239.255.255.250:3702 224.0.0.252:5355 224.0.0.252:5355 224.0.0.252:5355 224.0.0.252:5355 8.8.8.8:53 8.8.8.8:53 224.0.0.252:5355 224.0.0.252:5355 224.0.0.252:5355 224.0.0.252:5355 8.8.8.8:53 8.8.8.8:53 224.0.0.252:5355 224.0.0.252:5355 224.0.0.252:5355 224.0.0.252:5355 8.8.8.8:53 8.8.8.8:53 224.0.0.252:5355 224.0.0.252:5355 224.0.0.252:5355 224.0.0.252:5355 224.0.0.252:5355 224.0.0.252:5355 8.8.8.8:53 8.8.8.8:53 8.8.8.8:53 8.8.8.8:53 8.8.8.8:53</t>
-  </si>
-  <si>
-    <t>onlinegames</t>
-  </si>
-  <si>
-    <t>0270649e60d890ee82bd52c31fa25895</t>
-  </si>
-  <si>
-    <t>LdrLoadDll LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrLoadDll LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrLoadDll LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrLoadDll LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrLoadDll LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress NtProtectVirtualMemory NtProtectVirtualMemory GetCursorPos SetErrorMode SetErrorMode FindResourceA FindResourceA SetWindowsHookExA FindResourceA FindResourceA LoadResource SetWindowsHookExA NtAllocateVirtualMemory NtFreeVirtualMemory NtAllocateVirtualMemory LdrGetDllHandle LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetDllHandle LdrGetProcedureAddress LdrGetDllHandle LdrGetProcedureAddress LdrGetDllHandle LdrGetProcedureAddress LdrGetDllHandle LdrGetProcedureAddress LdrGetDllHandle LdrGetProcedureAddress LdrGetDllHandle LdrGetProcedureAddress LdrGetDllHandle LdrGetProcedureAddress LdrGetDllHandle LdrGetProcedureAddress LdrGetDllHandle LdrGetProcedureAddress LdrGetDllHandle LdrGetProcedureAddress LdrGetDllHandle LdrGetProcedureAddress LdrGetDllHandle LdrGetProcedureAddress LdrGetDllHandle LdrGetProcedureAddress LdrGetDllHandle LdrGetProcedureAddress LdrGetDllHandle LdrGetProcedureAddress LdrGetDllHandle LdrGetProcedureAddress LdrGetDllHandle LdrGetProcedureAddress LdrGetDllHandle LdrGetProcedureAddress LdrGetDllHandle LdrGetProcedureAddress LdrGetDllHandle LdrGetProcedureAddress LdrGetDllHandle LdrGetProcedureAddress LdrGetDllHandle LdrGetProcedureAddress LdrGetDllHandle LdrGetProcedureAddress LdrGetDllHandle LdrGetProcedureAddress LdrGetDllHandle LdrGetProcedureAddress LdrGetDllHandle LdrGetProcedureAddress LdrGetProcedureAddress NtAllocateVirtualMemory NtAllocateVirtualMemory LdrGetDllHandle LdrGetDllHandle LdrGetProcedureAddress NtOpenProcess NtClose GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics NtClose NtOpenKey GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics RegCloseKey GetSystemMetrics GetSystemMetrics GetSystemMetrics LdrLoadDll LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrLoadDll LdrGetProcedureAddress LdrLoadDll LdrGetProcedureAddress LdrUnloadDll LdrLoadDll LdrGetProcedureAddress LdrUnloadDll LdrLoadDll LdrGetProcedureAddress LdrUnloadDll LdrLoadDll LdrGetProcedureAddress LdrUnloadDll LdrLoadDll LdrGetProcedureAddress LdrUnloadDll GetSystemMetrics NtClose NtOpenKey NtQueryValueKey NtClose NtOpenKey NtQueryValueKey NtClose NtAllocateVirtualMemory NtFreeVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtOpenKey NtOpenKey NtOpenKey NtQueryValueKey NtQueryValueKey GetForegroundWindow NtClose NtClose GetSystemMetrics NtAllocateVirtualMemory GetSystemMetrics GetSystemMetrics LdrLoadDll LdrGetProcedureAddress FindResourceA FindResourceA FindResourceA FindResourceA FindResourceA FindResourceA LdrGetDllHandle LdrGetProcedureAddress LookupPrivilegeValueW NtClose GetTempPathW FindResourceA LoadResource GetFileAttributesW NtCreateFile LdrGetDllHandle LdrGetProcedureAddress SizeofResource NtWriteFile NtClose FindResourceA LoadResource GetFileAttributesW NtCreateFile LdrGetDllHandle LdrGetProcedureAddress SizeofResource NtWriteFile NtClose NtOpenMutant FindResourceA LoadResource GetFileAttributesW NtCreateFile LdrGetDllHandle LdrGetProcedureAddress SizeofResource NtWriteFile NtClose GetShortPathNameW NtOpenFile NtClose CreateProcessInternalW NtClose NtClose NtCreateFile GetFileType NtWriteFile NtClose RegOpenKeyExA RegSetValueExA RegCloseKey RegOpenKeyExA RegSetValueExA RegCloseKey RegCreateKeyExA RegSetValueExA RegCloseKey RegCreateKeyExA RegSetValueExA RegCloseKey CreateProcessInternalW NtClose NtClose OutputDebugStringA NtCreateFile LdrGetDllHandle LdrGetProcedureAddress NtWriteFile NtClose CreateProcessInternalW NtClose NtClose GetSystemTimeAsFileTime RegOpenKeyExA RegQueryValueExA RegCloseKey RegOpenKeyExA RegQueryValueExA RegCloseKey RegOpenKeyExW RegQueryValueExW RegCloseKey CreateThread NtClose LdrLoadDll NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory LdrGetDllHandle LdrGetProcedureAddress CreateThread NtClose LdrLoadDll LdrLoadDll LdrGetProcedureAddress LdrGetProcedureAddress GetSystemWindowsDirectoryW NtCreateFile NtCreateSection NtMapViewOfSection NtClose NtClose FindResourceA FindResourceA LoadResource LdrGetDllHandle LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrLoadDll LdrGetProcedureAddress NtCreateFile LdrLoadDll CreateThread NtDeviceIoControlFile NtDeviceIoControlFile NtDeviceIoControlFile LdrGetDllHandle LdrGetProcedureAddress LdrGetDllHandle LdrGetProcedureAddress CreateThread NtClose NtDeviceIoControlFile NtDeviceIoControlFile NtDelayExecution LdrUnloadDll DrawTextExW GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics UnhookWindowsHookEx UnhookWindowsHookEx LdrGetDllHandle LdrGetDllHandle NtTerminateProcess NtTerminateProcess NtClose NtClose NtClose NtClose NtClose NtClose NtClose LdrGetDllHandle LdrGetProcedureAddress LdrGetDllHandle LdrGetProcedureAddress NtClose LdrGetDllHandle LdrUnloadDll NtClose LdrUnloadDll NtOpenKey NtQueryValueKey NtClose NtClose NtClose NtClose NtClose NtTerminateProcess</t>
-  </si>
-  <si>
-    <t>192.168.56.101:49360 192.168.56.101:64412 192.168.56.101:50300 192.168.56.101:137 192.168.56.101:1900 192.168.56.101:49362 192.168.56.101:58084 192.168.56.101:58085 192.168.56.101:54425 192.168.56.101:138 192.168.56.101:52057 192.168.56.101:59469 192.168.56.101:54227 192.168.56.101:54228 192.168.56.101:52887 192.168.56.101:63529 192.168.56.101:51765 192.168.56.101:49465 192.168.56.101:50974 192.168.56.101:55167</t>
-  </si>
-  <si>
-    <t>224.0.0.252:5355 8.8.8.8:53 239.255.255.250:3702 192.168.56.255:137 239.255.255.250:1900 239.255.255.250:1900 224.0.0.252:5355 239.255.255.250:3702 8.8.8.8:53 192.168.56.255:138 224.0.0.252:5355 224.0.0.252:5355 224.0.0.252:5355 239.255.255.250:3702 224.0.0.252:5355 8.8.8.8:53 224.0.0.252:5355 224.0.0.252:5355 224.0.0.252:5355 8.8.8.8:53</t>
+    <t>fareit</t>
+  </si>
+  <si>
+    <t>008cd3997b67450340a5b32b0346e6db</t>
+  </si>
+  <si>
+    <t>RegOpenKeyExA RegOpenKeyExA RegOpenKeyExA NtOpenKey NtQueryValueKey NtClose NtOpenKey NtQueryValueKey NtClose NtClose NtQueryAttributesFile NtQueryAttributesFile NtQueryAttributesFile NtQueryAttributesFile LoadStringA LoadStringA LoadStringA LoadStringA LoadStringA LoadStringA LoadStringA LoadStringA LoadStringA LoadStringA LoadStringA LoadStringA LoadStringA LoadStringA LoadStringA LoadStringA LoadStringA LoadStringA LoadStringA LoadStringA LoadStringA LoadStringA LoadStringA LoadStringA LoadStringA LoadStringA LoadStringA LoadStringA LoadStringA NtAllocateVirtualMemory NtAllocateVirtualMemory LoadStringA LoadStringA LdrGetDllHandle LdrGetProcedureAddress LdrGetDllHandle LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetDllHandle LoadStringA LoadStringA LoadStringA LoadStringA LoadStringA LoadStringA LoadStringA LoadStringA LoadStringA LoadStringA LoadStringA LoadStringA LoadStringA LoadStringA LoadStringA LoadStringA LoadStringA LoadStringA LdrGetProcedureAddress LdrGetProcedureAddress GetSystemMetrics GetSystemMetrics FindResourceExW LoadResource FindResourceExW LoadResource FindResourceExW LoadResource FindResourceExW LoadResource FindResourceExW LoadResource FindResourceExW LoadResource FindResourceExW LoadResource FindResourceExW LoadResource FindResourceExW LoadResource FindResourceExW LoadResource FindResourceExW LoadResource FindResourceExW LoadResource FindResourceExW LoadResource FindResourceExW LoadResource LdrGetProcedureAddress FindResourceExW LoadResource FindResourceExW LoadResource NtAllocateVirtualMemory GetSystemMetrics GetSystemMetrics NtClose NtClose GetSystemMetrics NtAllocateVirtualMemory GetSystemMetrics GetSystemMetrics LdrLoadDll LdrGetProcedureAddress LdrGetDllHandle FindResourceExW LoadResource FindResourceExW LoadResource DrawTextExW GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics DrawTextExW LdrGetDllHandle FindResourceExW LoadResource FindResourceExW LoadResource FindResourceExW LoadResource LdrGetDllHandle LdrGetProcedureAddress LoadStringA LoadStringA LoadStringA LoadStringA LoadStringA LoadStringA LoadStringA LoadStringA LoadStringA LoadStringA LoadStringA LoadStringA LoadStringA LoadStringA LoadStringA LoadStringA LoadStringA LoadStringA LoadStringA LoadStringA LoadStringA LoadStringA LoadStringA LoadStringA LoadStringA LoadStringA LoadStringA LoadStringA LoadStringA LoadStringA LoadStringA LoadStringA LoadStringA LoadStringA LoadStringA LoadStringA LoadStringA LoadStringA LoadStringA LoadStringA LoadStringA LoadStringA LoadStringA LoadStringA LoadStringA LoadStringA LoadStringA LdrGetDllHandle LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetDllHandle LdrGetProcedureAddress GetSystemMetrics GetSystemMetrics FindResourceA FindResourceA LoadResource SizeofResource NtAllocateVirtualMemory NtAllocateVirtualMemory LdrLoadDll LdrGetProcedureAddress LdrGetProcedureAddress GetSystemWindowsDirectoryW NtCreateFile NtCreateSection NtMapViewOfSection NtClose NtClose GetSystemMetrics NtAllocateVirtualMemory CreateActCtxW GetSystemWindowsDirectoryW CreateActCtxW LdrGetDllHandle LdrGetProcedureAddress LdrLoadDll LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrLoadDll LdrGetProcedureAddress GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics LdrGetProcedureAddress GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics FindResourceExW LoadResource GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics NtAllocateVirtualMemory LdrLoadDll LdrGetProcedureAddress LdrGetProcedureAddress LdrLoadDll NtQuerySystemInformation RegOpenKeyExA RegQueryValueExA RegCloseKey NtOpenKey NtQueryValueKey NtClose NtOpenKey NtQueryValueKey NtClose NtOpenKey NtQueryValueKey NtClose RegOpenKeyExW GlobalMemoryStatusEx NtOpenKey NtOpenKey NtQueryValueKey NtClose LdrGetProcedureAddress NtDuplicateObject LdrGetProcedureAddress LdrLoadDll LdrGetProcedureAddress NtCreateThreadEx NtDuplicateObject NtResumeThread LdrGetProcedureAddress LdrGetProcedureAddress NtClose NtOpenKey NtClose NtOpenKey NtQueryValueKey NtQueryValueKey NtClose RegOpenKeyExW RegQueryValueExW RegCloseKey LdrLoadDll NtOpenProcess NtClose NtCreateMutant LdrGetProcedureAddress GetSystemTimeAsFileTime GetSystemTimeAsFileTime GetSystemTimeAsFileTime GetSystemTimeAsFileTime GetSystemTimeAsFileTime GetSystemTimeAsFileTime GetSystemTimeAsFileTime GetSystemTimeAsFileTime GetSystemWindowsDirectoryW CreateProcessInternalW GetSystemTimeAsFileTime GetSystemTimeAsFileTime GetSystemTimeAsFileTime GetSystemTimeAsFileTime GetSystemTimeAsFileTime GetSystemTimeAsFileTime GetSystemTimeAsFileTime GetSystemTimeAsFileTime GetSystemTimeAsFileTime GetSystemTimeAsFileTime GetSystemTimeAsFileTime GetSystemTimeAsFileTime GetSystemTimeAsFileTime GetSystemTimeAsFileTime GetSystemTimeAsFileTime GetSystemTimeAsFileTime NtClose NtClose NtClose NtClose LdrUnloadDll LdrLoadDll NtOpenProcess NtClose NtCreateMutant NtClose NtClose LdrUnloadDll LdrLoadDll NtOpenProcess NtClose NtCreateMutant NtClose NtClose LdrUnloadDll FindResourceExW LoadResource FindResourceExW LoadResource FindResourceExW LoadResource FindResourceExW LoadResource FindResourceExW LoadResource FindResourceExW LoadResource FindResourceExW LoadResource FindResourceExW LoadResource FindResourceExW LoadResource FindResourceExW LoadResource FindResourceExW LoadResource FindResourceExW LoadResource FindResourceExW LoadResource FindResourceExW LoadResource FindResourceExW LoadResource FindResourceExW LoadResource FindResourceExW LoadResource FindResourceExW LoadResource FindResourceExW LoadResource FindResourceExW LoadResource FindResourceExW LoadResource FindResourceExW LoadResource FindResourceExW LoadResource FindResourceExW LoadResource LdrLoadDll LdrGetProcedureAddress NtClose NtOpenKey RegOpenKeyExW LdrLoadDll LdrGetProcedureAddress NtClose RegOpenKeyExW RegQueryValueExW RegCloseKey RegCloseKey LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrLoadDll NtOpenProcess NtClose NtCreateMutant NtClose NtClose LdrUnloadDll LdrLoadDll NtOpenProcess NtClose NtCreateMutant NtClose NtClose LdrUnloadDll LoadStringW FindResourceExW LoadResource EnumWindows GetSystemMetrics NtAllocateVirtualMemory GetSystemMetrics LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrLoadDll NtOpenProcess NtClose NtCreateMutant NtClose CreateThread NtClose NtClose NtClose LdrGetProcedureAddress LdrLoadDll LdrUnloadDll LdrGetProcedureAddress LdrLoadDll LdrUnloadDll LdrGetProcedureAddress LdrLoadDll LdrUnloadDll LdrGetProcedureAddress LdrLoadDll LdrUnloadDll GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics NtOpenSection NtMapViewOfSection RegOpenKeyExW RegQueryValueExW RegCloseKey RegOpenKeyExW LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrLoadDll LdrUnloadDll LdrLoadDll LdrUnloadDll LdrLoadDll LdrUnloadDll LdrLoadDll LdrUnloadDll LdrLoadDll LdrUnloadDll LoadStringW LoadStringW GetKeyState LdrLoadDll LdrUnloadDll LdrLoadDll LdrUnloadDll LdrLoadDll LdrUnloadDll LdrLoadDll LdrUnloadDll LdrLoadDll LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress GetNativeSystemInfo NtOpenProcess NtClose NtCreateSection LdrLoadDll LdrUnloadDll NtClose NtAllocateVirtualMemory LdrLoadDll LdrUnloadDll LdrLoadDll LdrUnloadDll DrawTextExW GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics DrawTextExW GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics DrawTextExW GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics DrawTextExW NtClose NtClose RegOpenKeyExW GetSystemDirectoryW LdrLoadDll LdrGetProcedureAddress LdrGetProcedureAddress CoInitializeEx LdrGetProcedureAddress LdrGetProcedureAddress NtClose NtClose RegOpenKeyExW RegQueryValueExW RegCloseKey NtClose NtClose NtClose NtClose NtClose NtClose GetSystemMetrics NtOpenMutant NtClose NtOpenMutant NtClose RegOpenKeyExW RegQueryValueExW RegCloseKey LdrGetDllHandle FindResourceExW FindResourceExW RegOpenKeyExW DrawTextExW GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics DrawTextExW DrawTextExW GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics DrawTextExW RegOpenKeyExW GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics LdrLoadDll LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress GetFileVersionInfoSizeW GetFileVersionInfoW DrawTextExW GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics DrawTextExW GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics DrawTextExW GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics DrawTextExW GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics DrawTextExW GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics DrawTextExW GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics DrawTextExW GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics DrawTextExW GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics DrawTextExW GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics DrawTextExW GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics DrawTextExW GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics DrawTextExW GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics DrawTextExW GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics DrawTextExW GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics DrawTextExW GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics DrawTextExW GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics DrawTextExW GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics DrawTextExW GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics DrawTextExW GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics DrawTextExW GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics DrawTextExW GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics DrawTextExW GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics DrawTextExW GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics DrawTextExW GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics DrawTextExW DrawTextExW GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics DrawTextExW GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics DrawTextExW DrawTextExW DrawTextExW GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics DrawTextExW GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics DrawTextExW DrawTextExW DrawTextExW DrawTextExW GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics DrawTextExW GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics DrawTextExW DrawTextExW DrawTextExW DrawTextExW DrawTextExW GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics DrawTextExW GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics NtAllocateVirtualMemory DrawTextExW DrawTextExW DrawTextExW DrawTextExW DrawTextExW DrawTextExW GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics DrawTextExW GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics FindResourceA FindResourceA LoadResource SizeofResource NtFreeVirtualMemory NtFreeVirtualMemory DrawTextExA GetCursorPos GetCursorPos GetSystemMetrics FindResourceExW FindResourceExW GetSystemMetrics GetSystemMetrics DrawTextExW GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics DrawTextExW GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics DrawTextExW GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics DrawTextExW GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics FindResourceExW LoadResource DrawTextExW GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics DrawTextExW GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics DrawTextExW GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics DrawTextExW GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics DrawTextExW GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics DrawTextExW GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics DrawTextExW GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics DrawTextExW GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics DrawTextExW DrawTextExW GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics DrawTextExW GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics DrawTextExW GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics DrawTextExW GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics DrawTextExW GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics DrawTextExW GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics DrawTextExW GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics DrawTextExW GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics DrawTextExA GetCursorPos NtCreateFile NtQueryInformationFile NtAllocateVirtualMemory NtAllocateVirtualMemory NtReadFile NtWriteFile NtSetInformationFile NtFreeVirtualMemory NtClose NtCreateFile NtQueryInformationFile NtAllocateVirtualMemory NtAllocateVirtualMemory NtReadFile NtWriteFile NtSetInformationFile NtFreeVirtualMemory NtClose NtCreateFile NtQueryInformationFile NtAllocateVirtualMemory NtAllocateVirtualMemory NtReadFile NtWriteFile NtSetInformationFile NtFreeVirtualMemory NtClose NtCreateFile NtQueryInformationFile NtAllocateVirtualMemory NtAllocateVirtualMemory NtReadFile NtWriteFile NtSetInformationFile NtFreeVirtualMemory NtClose NtCreateFile NtQueryInformationFile NtAllocateVirtualMemory NtAllocateVirtualMemory NtReadFile NtWriteFile NtSetInformationFile NtFreeVirtualMemory NtClose __exception__ FindResourceA FindResourceA SizeofResource LoadResource NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtFreeVirtualMemory NtFreeVirtualMemory NtFreeVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtDuplicateObject NtClose NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtua</t>
+  </si>
+  <si>
+    <t>192.168.56.101:49360 192.168.56.101:55311 192.168.56.101:137 192.168.56.101:64412 192.168.56.101:58084 192.168.56.101:54425 192.168.56.101:52057 192.168.56.101:59469 192.168.56.101:54227 192.168.56.101:123 192.168.56.101:1900</t>
+  </si>
+  <si>
+    <t>224.0.0.252:5355 239.255.255.250:1900 192.168.56.255:137 224.0.0.252:5355 224.0.0.252:5355 8.8.8.8:53 224.0.0.252:5355 224.0.0.252:5355 8.8.8.8:53 13.65.88.161:123 239.255.255.250:1900</t>
+  </si>
+  <si>
+    <t>softcnapp</t>
+  </si>
+  <si>
+    <t>0271c5b2484ec857619b56cbeaa5e438</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GetSystemTimeAsFileTime LdrLoadDll LdrLoadDll LdrGetProcedureAddress LdrLoadDll LdrGetProcedureAddress LdrGetProcedureAddress LdrLoadDll LdrGetProcedureAddress LdrGetProcedureAddress LdrLoadDll LdrLoadDll LdrGetProcedureAddress LdrLoadDll LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrLoadDll LdrGetProcedureAddress LdrGetDllHandle LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetDllHandle LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress SetUnhandledExceptionFilter LdrLoadDll LdrGetProcedureAddress LdrGetProcedureAddress NtOpenKey NtQueryValueKey NtClose NtOpenKey NtQueryValueKey NtClose NtOpenKey NtQueryValueKey NtClose NtOpenKey NtQueryValueKey NtClose LdrGetProcedureAddress NtClose NtOpenKey NtQueryValueKey NtClose NtOpenKey NtQueryValueKey NtClose NtOpenKey NtQueryValueKey NtClose NtOpenKey NtQueryValueKey NtClose NtOpenKey NtQueryValueKey NtClose NtOpenKey NtQueryValueKey NtClose NtOpenKey NtQueryValueKey NtClose NtOpenKey NtQueryValueKey NtClose NtOpenKey NtQueryValueKey NtClose NtOpenKey NtQueryValueKey NtClose NtOpenKey NtQueryValueKey NtClose NtOpenKey NtQueryValueKey NtClose NtOpenKey NtQueryValueKey NtClose NtOpenKey NtQueryValueKey NtClose NtOpenKey NtQueryValueKey GetFileAttributesW SHGetFolderPathW SHGetFolderPathW SetErrorMode GetFileAttributesW SetErrorMode SetErrorMode GetFileAttributesW SetErrorMode SetErrorMode GetFileAttributesW SetErrorMode SetErrorMode GetFileAttributesW SetErrorMode NtAllocateVirtualMemory SetErrorMode GetFileAttributesW SetErrorMode SetErrorMode GetFileAttributesW SetErrorMode SetErrorMode GetFileAttributesW SetErrorMode SetErrorMode GetFileAttributesW SetErrorMode SetErrorMode GetFileAttributesW SetErrorMode SetErrorMode GetFileAttributesW SetErrorMode CreateDirectoryW LdrLoadDll GetSystemTimeAsFileTime GetTimeZoneInformation NtCreateFile DeviceIoControl DeviceIoControl NtClose NtCreateFile NtCreateFile NtCreateFile NtCreateFile NtCreateFile NtCreateFile NtCreateFile NtCreateFile NtCreateFile NtCreateFile NtCreateFile NtCreateFile NtCreateFile NtCreateFile NtCreateFile GetAdaptersInfo GetAdaptersInfo GetSystemDirectoryW NtOpenFile NtQueryInformationFile NtClose CoInitializeEx WSAStartup GetSystemTimeAsFileTime LdrLoadDll GetSystemTimeAsFileTime LdrLoadDll CoCreateInstance NtClose NtClose GetSystemMetrics NtAllocateVirtualMemory GetSystemMetrics GetSystemMetrics LdrLoadDll LdrGetProcedureAddress GetSystemMetrics GetSystemMetrics NtClose NtClose RegOpenKeyExW GetSystemDirectoryW LdrLoadDll LdrGetProcedureAddress LdrGetProcedureAddress CoInitializeEx LdrGetProcedureAddress LdrGetProcedureAddress NtClose NtClose RegOpenKeyExW RegQueryValueExW RegCloseKey NtClose NtClose NtClose NtClose NtClose NtClose GetSystemMetrics NtOpenMutant NtClose NtOpenMutant NtClose NtAllocateVirtualMemory NtAllocateVirtualMemory RegOpenKeyExW RegQueryValueExW RegCloseKey RegOpenKeyExW NtAllocateVirtualMemory LdrGetDllHandle FindResourceExW FindResourceExW LdrLoadDll LdrLoadDll FindResourceW LoadResource SizeofResource NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtFreeVirtualMemory NtAllocateVirtualMemory GetSystemInfo LdrGetDllHandle LdrGetProcedureAddress LdrGetDllHandle LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress GetSystemMetrics GetSystemMetrics GetSystemMetrics LdrGetDllHandle LdrGetProcedureAddress LdrGetProcedureAddress GetSystemDirectoryW LdrLoadDll CreateThread GetSystemMetrics GetSystemMetrics FindResourceExW LoadResource FindResourceExW LoadResource LdrGetDllHandle GetSystemMetrics GetSystemMetrics FindResourceExW LoadResource FindResourceExW LoadResource NtFreeVirtualMemory NtFreeVirtualMemory NtFreeVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtFreeVirtualMemory NtAllocateVirtualMemory NtFreeVirtualMemory NtAllocateVirtualMemory NtFreeVirtualMemory NtFreeVirtualMemory NtFreeVirtualMemory NtFreeVirtualMemory NtFreeVirtualMemory NtFreeVirtualMemory LdrGetDllHandle LdrGetProcedureAddress CoCreateInstance NtAllocateVirtualMemory GetSystemMetrics GetSystemMetrics NtAllocateVirtualMemory FindResourceExW NtClose NtClose RegOpenKeyExW LdrLoadDll LdrLoadDll FindResourceW LoadResource SizeofResource NtAllocateVirtualMemory NtAllocateVirtualMemory GetSystemMetrics GetSystemMetrics FindResourceExW LoadResource FindResourceExW LoadResource LdrGetDllHandle GetSystemMetrics GetSystemMetrics FindResourceExW LoadResource FindResourceExW LoadResource CreateToolhelp32Snapshot Process32FirstW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW NtClose CreateToolhelp32Snapshot Process32FirstW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW NtClose CreateToolhelp32Snapshot Process32FirstW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW NtClose CreateToolhelp32Snapshot Process32FirstW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW NtClose CreateToolhelp32Snapshot Process32FirstW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW NtClose CreateToolhelp32Snapshot Process32FirstW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW NtClose CreateToolhelp32Snapshot Process32FirstW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW NtClose CreateToolhelp32Snapshot Process32FirstW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW NtClose CreateToolhelp32Snapshot Process32FirstW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW NtClose CreateToolhelp32Snapshot Process32FirstW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW NtClose NtFreeVirtualMemory NtFreeVirtualMemory NtFreeVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory CoCreateInstance SetWindowsHookExW SetWindowsHookExW NtOpenSection NtMapViewOfSection LdrLoadDll LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetDllHandle LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress RegOpenKeyExW RegQueryValueExW RegOpenKeyExW RegQueryValueExW RegOpenKeyExW RegQueryValueExW RegOpenKeyExW RegQueryValueExW LdrGetDllHandle LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegQueryValueExW RegQueryValueExW RegOpenKeyExW RegQueryValueExW RegCloseKey RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegCloseKey RegCloseKey RegCloseKey RegCloseKey RegOpenKeyExW RegQueryValueExW RegOpenKeyExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW NtClose RegOpenKeyExW RegOpenKeyExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegOpenKeyExW RegQueryValueExW RegCloseKey LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress RegOpenKeyExW RegQueryValueExW RegCloseKey RegOpenKeyExW RegOpenKeyExW RegQueryValueExW RegCloseKey RegOpenKeyExW RegOpenKeyExW RegQueryValueExW RegCloseKey RegOpenKeyExW RegOpenKeyExW RegQueryValueExW RegCloseKey RegOpenKeyExW RegOpenKeyExW RegQueryValueExW RegCloseKey RegOpenKeyExW RegOpenKeyExA LdrGetProcedureAddress LdrGetProcedureAddress LdrLoadDll LdrGetProcedureAddress RegOpenKeyExW RegQueryValueExW RegCloseKey RegOpenKeyExW RegOpenKeyExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegCloseKey RegOpenKeyExW RegQueryValueExW RegCloseKey RegOpenKeyExW RegOpenKeyExW RegQueryValueExW RegCloseKey RegOpenKeyExW RegQueryValueExW RegQueryValueExW RegCloseKey RegOpenKeyExW RegOpenKeyExW NtOpenKey NtQueryValueKey NtClose LdrGetDllHandle RegOpenKeyExW RegCloseKey RegOpenKeyExW RegQueryValueExW RegCloseKey NtOpenKey NtOpenKey NtQueryValueKey NtClose CoCreateInstance RegOpenKeyExA RegOpenKeyExW RegQueryValueExW RegCloseKey RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegCloseKey RegCloseKey RegCloseKey RegCloseKey RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegQueryValueExW RegCloseKey RegOpenKeyExW FindResourceExW LoadResource FindResourceExW LoadResource FindResourceExW LoadResource FindResourceExW LoadResource FindResourceExW LoadResource FindResourceExW LoadResource FindResourceExW LoadResource FindResourceExW LoadResource FindResourceExW LoadResource FindResourceExW LoadResource FindResourceExW LoadResource FindResourceExW LoadResource FindResourceExW LoadResource FindResourceExW LoadResource FindResourceExW LoadResource FindResourceExW LoadResource FindResourceExW LoadResource FindResourceExW LoadResource FindResourceExW LoadResource FindResourceExW LoadResource FindResourceExW LoadResource FindResourceExW LoadResource FindResourceExW LoadResource FindResourceExW LoadResource FindResourceExW LoadResource FindResourceExW LoadResource FindResourceExW LoadResource FindResourceExW LoadResource FindResourceExW LoadResource FindResourceExW LoadResource FindResourceExW LoadResource FindResourceExW LoadResource FindResourceExW LoadResource FindResourceExW LoadResource FindResourceExW LoadResource FindResourceExW LoadResource FindResourceExW LoadResource CoInitializeEx CoUninitialize LdrGetProcedureAddress RegOpenKeyExA RegOpenKeyExA RegOpenKeyExA RegCloseKey RegOpenKeyExW RegOpenKeyExW RegQueryValueExA RegCloseKey NtOpenSection NtQueryAttributesFile NtQueryAttributesFile NtOpenFile NtCreateSection NtMapViewOfSection NtClose NtClose NtProtectVirtualMemory NtOpenSection NtMapViewOfSection NtClose NtProtectVirtualMemory NtProtectVirtualMemory NtProtectVirtualMemory GetSystemTimeAsFileTime GetSystemTimeAsFileTime RegOpenKeyExW RegQueryValueExW RegCloseKey RegOpenKeyExW RegQueryValueExW RegCloseKey RegOpenKeyExW RegQueryValueExW RegCloseKey CoGetClassObject LdrGetProcedureAddress LdrGetProcedureAddress RegOpenKeyExW RegOpenKeyExA RegEnumValueA RegEnumValueA RegEnumValueA RegEnumValueA RegEnumValueA RegEnumValueA RegEnumValueA RegEnumValueA RegEnumValueA RegEnumValueA RegEnumValueA RegEnumValueA RegEnumValueA LdrGetProcedureAddress RegCloseKey RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegQueryValueExA RegCloseKey CoGetClassObject RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegCloseKey RegCloseKey RegCloseKey RegCloseKey LdrGetProcedureAddress RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegQueryInfoKeyW RegCloseKey RegOpenKeyExW RegQueryInfoKeyW RegCloseKey RegOpenKeyExW RegQueryValueExW RegCloseKey LdrGetProcedureAddress RegOpenKeyExW RegQueryValueExW RegCloseKey RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegCloseKey RegCloseKey RegCloseKey RegCloseKey RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegQueryValueExW RegQueryValueExW NtCreateMutant RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegCloseKey RegCloseKey RegCloseKey RegCloseKey RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegQueryInfoKeyW RegCloseKey RegOpenKeyExW RegQueryInfoKeyW RegEnumValueW RegEnumValueW RegEnumValueW RegEnumValueW RegEnumValueW RegEnumValueW RegEnumValueW RegCloseKey RegOpenKeyExW RegQueryInfoKeyW RegCloseKey RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegQueryValueExW RegCloseKey RegOpenKeyExW RegQueryValueExW RegCloseKey GetUserNameW NtCreateSection NtMapViewOfSection NtCreateMutant RegOpenKeyExW RegQueryValueExW RegCloseKey RegOpenKeyExW RegOpenKeyExW RegCloseKey RegOpenKeyExW RegCloseKey RegOpenKeyExW RegCloseKey RegOpenKeyExW RegCloseKey RegOpenKeyExW RegCloseKey RegCloseKey RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegEnumKeyExW NtCreateMutant RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegQueryValueExW RegCloseKey RegCloseKey RegEnumKeyExW RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegQueryValueExW RegOpenKeyExW RegDeleteValueW RegOpenKeyExW RegDeleteValueW RegDeleteValueW RegDeleteValueW RegSetValueExW RegSetValueExW RegCloseKey RegCloseKey RegCloseKey RegCloseKey RegEnumKeyExW RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegQueryValueExW RegCloseKey RegCloseKey RegEnumKeyExW RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegQueryValueExW RegCloseKey RegCloseKey RegEnumKeyExW RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegQueryValueExW RegCloseKey RegCloseKey RegEnumKeyExW RegCloseKey RegOpenKeyExW RegQueryValueExW RegQueryValueExW RegOpenKeyExW RegQueryValueExW RegQueryValueExW NtCreateMutant RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegEnumKeyExW NtCreateMutant RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegQueryValueExW RegCloseKey RegCloseKey RegEnumKeyExW RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegQueryValueExW RegOpenKeyExW RegDeleteValueW RegOpenKeyExW RegDeleteValueW RegDeleteValueW RegDeleteValueW RegSetValueExW RegSetValueExW RegCloseKey RegCloseKey RegCloseKey RegCloseKey RegEnumKeyExW RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegQueryValueExW RegCloseKey RegCloseKey RegEnumKeyExW RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegQueryValueExW RegCloseKey RegCloseKey RegEnumKeyExW RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegQueryValueExW RegCloseKey RegCloseKey RegEnumKeyExW RegCloseKey RegOpenKeyExW RegOpenKeyExW RegQueryValueExA RegCloseKey CoGetClassObject RegOpenKeyExW RegOpenKeyExW RegQueryValueExA RegCloseKey CoGetClassObject RegCloseKey RegCloseKey RegOpenKeyExW RegQueryValueExW RegOpenKeyExW RegQueryValueExW RegOpenKeyExW RegQueryValueExW RegOpenKeyExW RegQueryValueExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegOpenKeyExW RegOpenKeyExW RegQueryValueExA RegCloseKey CoGetClassObject RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegQueryValueExW RegOpenKeyExW RegOpenKeyExW RegQueryValueExA RegCloseKey CoGetClassObject GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics RegCloseKey GetSystemWindowsDirectoryW CreateActCtxW LdrLoadDll LdrGetDllHandle LdrLoadDll LdrGetProcedureAddress LdrGetProcedureAddress NtUnmapViewOfSection NtClose RegOpenKeyExW RegQueryValueExW RegCloseKey RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegQueryValueExW RegQueryValueExW RegCloseKey RegCloseKey RegCloseKey RegCloseKey RegCloseKey RegOpenKeyExW RegOpenKeyExW RegQueryValueExA RegCloseKey CoGetClassObject RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegQueryValueExW RegOpenKeyExA RegQueryValueExA RegCloseKey RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegQueryValueExW RegOpenKeyExW RegQueryValueExW RegCloseKey RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegCloseKey RegCloseKey RegCloseKey RegCloseKey RegOpenKeyExW RegCloseKey RegOpenKeyExW RegQueryValueExW RegCloseKey LoadStringW RegOpenKeyExW RegQueryValueExW RegCloseKey LoadStringW RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegQueryValueExW CoGetClassObject GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics RegCloseKey GetSystemWindowsDirectoryW CreateActCtxW NtClose NtOpenKey NtClose NtOpenKey NtQueryValueKey NtClose NtClose NtOpenKey NtClose NtOpenKey NtQueryValueKey NtClose NtClose NtOpenKey NtClose NtOpenKey NtQueryValueKey NtClose NtClose NtOpenKey NtClose NtOpenKey NtQueryValueKey NtClose ReadProcessMemory ReadProcessMemory ReadProcessMemory ReadProcessMemory ReadProcessMemory RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegCloseKey RegCloseKey RegCloseKey RegCloseKey RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegQueryValueExW RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegQueryValueExW RegCloseKey RegOpenKeyExW RegQueryValueExW RegCloseKey RegOpenKeyExW RegOpenKeyExW RegQueryValueExA RegCloseKey CoGetClassObject RegOpenKeyExW RegOpenKeyExW RegQueryValueExA RegCloseKey CoGetClassObject RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegCloseKey RegCloseKey RegCloseKey RegCloseKey RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegQueryValueExW RegOpenKeyExW RegQueryValueExW RegCloseKey RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegCloseKey RegCloseKey RegCloseKey RegCloseKey LdrGetDllHandle LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress RegOpenKeyExW RegOpenKeyExW RegQueryValueExA RegCloseKey CoGetClassObject RegOpenKeyExW RegQueryValueExW RegOpenKeyExA RegOpenKeyExA RegOpenKeyExA RegCloseKey RegOpenKeyExW RegOpenKeyExW RegQueryValueExA RegCloseKey CoGetClassObject RegCloseKey RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegCloseKey RegCloseKey RegCloseKey RegCloseKey RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegQueryValueExW RegCloseKey RegOpenKeyExW RegQueryValueExW RegCloseKey RegCloseKey RegCloseKey RegOpenKeyExW RegCloseKey RegQueryValueExW RegQueryValueExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegOpenKeyExW RegOpenKeyExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegQueryValueExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegOpenKeyExW RegQueryValueExW RegOpenKeyExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegQueryValueExW RegQueryValueExW RegOpenKeyExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW LdrGetDllHandle LdrGetDllHandle LdrGetDllHandle LdrGetDllHandle RegOpenKeyExW RegQueryValueExW RegCloseKey RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegOpenKeyExA RegQueryValueExW RegCloseKey RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegCloseKey RegQueryInfoKeyW RegEnumValueW RegEnumValueW RegEnumValueW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegOpenKeyExW RegOpenKeyExW RegQueryValueExA RegCloseKey CoGetClassObject RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegQueryValueExW LdrGetProcedureAddress LdrGetProcedureAddress RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegQueryValueExW RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegQueryValueExW RegQueryValueExW RegCloseKey RegCloseKey RegCloseKey RegCloseKey RegCloseKey GetCursorPos GetKeyState GetKeyState GetKeyState GetKeyState GetKeyState GetKeyState LdrGetProcedureAddress RegOpenKeyExW RegQueryValueExW RegCloseKey NtAllocateVirtualMemory NtAllocateVirtualMemory LdrLoadDll LdrGetProcedureAddress LdrGetProcedureAddress RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegQueryValueExW RegQueryValueExW RegCloseKey RegCloseKey RegCloseKey RegCloseKey RegCloseKey RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegCloseKey RegCloseKey RegCloseKey RegCloseKey FindWindowW FindWindowW NtAllocateVirtualMemory CreateThread LdrGetProcedureAddress RegOpenKeyExW RegQueryValueExW RegCloseKey NtAllocateVirtualMemory RegOpenKeyExW RegQueryValueExW RegCloseKey RegOpenKeyExW RegOpenKeyExW RegQueryValueExW RegCloseKey LdrGetProcedureAddress RegOpenKeyExW RegQueryValueExW RegCloseKey RegOpenKeyExW RegQueryValueExW RegCloseKey NtAllocateVirtualMemory RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegCloseKey RegCloseKey RegCloseKey RegCloseKey LdrLoadDll CoInitializeEx LoadStringW LoadStringW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegCloseKey RegCloseKey RegOpenKeyExW RegOpenKeyExW LoadStringW LoadStringW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegCloseKey RegCloseKey RegOpenKeyExW RegQueryValueExW RegCloseKey RegOpenKeyExW RegQueryValueExW RegCloseKey RegOpenKeyExW RegOpenKeyExW LoadStringW LoadStringW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegCloseKey RegCloseKey RegOpenKeyExW RegQueryValueExW RegOpenKeyExW RegQueryValueExW RegCloseKey RegCloseKey RegOpenKeyExW RegQueryValueExW RegCloseKey RegOpenKeyExW RegOpenKeyExW LoadStringW LoadStringW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegCloseKey RegCloseKey RegOpenKeyExW RegQueryValueExW RegOpenKeyExW RegQueryValueExW RegCloseKey RegCloseKey RegOpenKeyExW RegQueryValueExW RegCloseKey RegOpenKeyExW RegOpenKeyExW LoadStringW LoadStringW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegCloseKey RegCloseKey RegOpenKeyExW RegQueryValueExW RegOpenKeyExW RegQueryValueExW RegCloseKey RegCloseKey RegOpenKeyExW RegQueryValueExW RegCloseKey LdrGetProcedureAddress RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegCloseKey RegCloseKey RegCloseKey RegCloseKey NtOpenMutant NtClose NtClose NtClose NtCreateMutant NtDuplicateObject NtClose RegOpenKeyExW RegCloseKey RegQueryValueExW RegQueryValueExW LdrLoadDll LdrGetProcedureAddress GetFileVersionInfoSizeW LdrGetProcedureAddress GetFileVersionInfoW LdrGetProcedureAddress NtClose RegQueryValueExW RegQueryValueExW GetUserNameA NtClose RegCreateKeyExA RegQueryValueExA LdrGetDllHandle LdrGetProcedureAddress RegOpenKeyExA RegQueryValueExA RegCloseKey RegOpenKeyExA RegOpenKeyExA RegOpenKeyExA RegQueryValueExA RegCloseKey RegOpenKeyExA RegQueryValueExA RegOpenKeyExA RegQueryValueExA RegCloseKey RegCloseKey RegOpenKeyExA LdrLoadDll LdrGetProcedureAddress SHGetFolderPathW GetFileAttributesW GetFileAttributesW GetFileAttributesW GetFileAttributesW GetFileAttributesW GetFileAttributesW RegQueryValueExA RegQueryValueExA RegOpenKeyExA RegQueryValueExA RegOpenKeyExA RegQueryValueExA RegCloseKey RegCloseKey RegCloseKey RegOpenKeyExA SHGetFolderPathW GetFileAttributesW RegQueryValueExA RegQueryValueExA RegOpenKeyExA RegQueryValueExA RegOpenKeyExA RegQueryValueExA RegCloseKey RegCloseKey RegCloseKey RegOpenKeyExA SHGetFolderPathW GetFileAttributesW GetFileAttributesW GetFileAttributesW GetFileAttributesW GetFileAttributesW GetFileAttributesW RegQueryValueExA RegQueryValueExA RegCloseKey RegCloseKey RegCloseKey NtOpenMutant NtOpenMutant GetFileAttributesW SetFileAttributesW NtCreateFile GetFileAttributesW SetFileTime GetFileSize NtOpenSection NtMapViewOfSection NtOpenMutant GetFileAttributesW SetFileAttributesW NtCreateFile GetFileAttributesW SetFileTime GetFileSize NtOpenSection NtMapViewOfSection NtOpenMutant GetFileAttributesW SetFileAttributesW NtCreateFile GetFileAttributesW SetFileTime GetFileSize NtOpenSection NtMapViewOfSection GetFileAttributesW GetFileAttributesW GetFileAttributesW GetFileAttributesW RegOpenKeyExA RegOpenKeyExA RegCloseKey RegEnumKeyExA RegOpenKeyExA RegQueryValueExA RegQueryValueExA RegQueryValueExA RegQueryValueExA RegQueryValueExA RegCloseKey RegEnumKeyExA RegOpenKeyExA RegQueryValueExA RegQueryValueExA RegQueryValueExA RegQueryValueExA RegQueryValueExA RegCloseKey RegEnumKeyExA RegOpenKeyExA RegQueryValueExA RegQueryValueExA RegQueryValueExA RegQueryValueExA RegQueryValueExA RegCloseKey RegEnumKeyExA RegOpenKeyExA RegQueryValueExA RegQueryValueExA RegQueryValueExA RegQueryValueExA RegQueryValueExA NtAllocateVirtualMemory RegCloseKey RegEnumKeyExA RegOpenKeyExA RegQueryValueExA RegQueryValueExA RegQueryValueExA RegQueryValueExA RegQueryValueExA RegCloseKey RegEnumKeyExA RegCloseKey NtOpenMutant NtCreateMutant GetFileAttributesW SetFileAttributesW NtCreateFile GetFileAttributesW SetFileTime GetFileSize NtOpenSection NtCreateSection NtMapViewOfSection RegOpenKeyExW RegQueryValueExW RegCloseKey NtAllocateVirtualMemory NtAllocateVirtualMemory CreateThread RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegQueryValueExW RegQueryValueExW RegCloseKey RegCloseKey RegCloseKey RegCloseKey </t>
+  </si>
+  <si>
+    <t>192.168.56.101:49360 192.168.56.101:50300 192.168.56.101:64412 192.168.56.101:137 192.168.56.101:1900 192.168.56.101:53352 192.168.56.101:64413 192.168.56.101:138 192.168.56.101:64415 192.168.56.101:58084 192.168.56.101:54425 192.168.56.101:52057 192.168.56.101:59469 192.168.56.101:54227 192.168.56.101:54228 192.168.56.101:54230 192.168.56.101:52887 192.168.56.101:63529 192.168.56.101:51765 192.168.56.101:49465 192.168.56.101:50974 192.168.56.101:55167 192.168.56.101:63794 192.168.56.101:62948 192.168.56.101:49746</t>
+  </si>
+  <si>
+    <t>8.8.8.8:53 239.255.255.250:3702 224.0.0.252:5355 192.168.56.255:137 239.255.255.250:1900 239.255.255.250:1900 239.255.255.250:3702 192.168.56.255:138 239.255.255.250:3702 224.0.0.252:5355 8.8.8.8:53 224.0.0.252:5355 224.0.0.252:5355 224.0.0.252:5355 239.255.255.250:3702 239.255.255.250:3702 224.0.0.252:5355 224.0.0.252:5355 224.0.0.252:5355 8.8.8.8:53 224.0.0.252:5355 8.8.8.8:53 8.8.8.8:53 224.0.0.252:5355 8.8.8.8:53</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
More preprocessing error handling
</commit_message>
<xml_diff>
--- a/data/test_data.xlsx
+++ b/data/test_data.xlsx
@@ -31,34 +31,34 @@
     <t>network_udp_dst</t>
   </si>
   <si>
-    <t>fareit</t>
-  </si>
-  <si>
-    <t>008cd3997b67450340a5b32b0346e6db</t>
-  </si>
-  <si>
-    <t>RegOpenKeyExA RegOpenKeyExA RegOpenKeyExA NtOpenKey NtQueryValueKey NtClose NtOpenKey NtQueryValueKey NtClose NtClose NtQueryAttributesFile NtQueryAttributesFile NtQueryAttributesFile NtQueryAttributesFile LoadStringA LoadStringA LoadStringA LoadStringA LoadStringA LoadStringA LoadStringA LoadStringA LoadStringA LoadStringA LoadStringA LoadStringA LoadStringA LoadStringA LoadStringA LoadStringA LoadStringA LoadStringA LoadStringA LoadStringA LoadStringA LoadStringA LoadStringA LoadStringA LoadStringA LoadStringA LoadStringA LoadStringA LoadStringA NtAllocateVirtualMemory NtAllocateVirtualMemory LoadStringA LoadStringA LdrGetDllHandle LdrGetProcedureAddress LdrGetDllHandle LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetDllHandle LoadStringA LoadStringA LoadStringA LoadStringA LoadStringA LoadStringA LoadStringA LoadStringA LoadStringA LoadStringA LoadStringA LoadStringA LoadStringA LoadStringA LoadStringA LoadStringA LoadStringA LoadStringA LdrGetProcedureAddress LdrGetProcedureAddress GetSystemMetrics GetSystemMetrics FindResourceExW LoadResource FindResourceExW LoadResource FindResourceExW LoadResource FindResourceExW LoadResource FindResourceExW LoadResource FindResourceExW LoadResource FindResourceExW LoadResource FindResourceExW LoadResource FindResourceExW LoadResource FindResourceExW LoadResource FindResourceExW LoadResource FindResourceExW LoadResource FindResourceExW LoadResource FindResourceExW LoadResource LdrGetProcedureAddress FindResourceExW LoadResource FindResourceExW LoadResource NtAllocateVirtualMemory GetSystemMetrics GetSystemMetrics NtClose NtClose GetSystemMetrics NtAllocateVirtualMemory GetSystemMetrics GetSystemMetrics LdrLoadDll LdrGetProcedureAddress LdrGetDllHandle FindResourceExW LoadResource FindResourceExW LoadResource DrawTextExW GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics DrawTextExW LdrGetDllHandle FindResourceExW LoadResource FindResourceExW LoadResource FindResourceExW LoadResource LdrGetDllHandle LdrGetProcedureAddress LoadStringA LoadStringA LoadStringA LoadStringA LoadStringA LoadStringA LoadStringA LoadStringA LoadStringA LoadStringA LoadStringA LoadStringA LoadStringA LoadStringA LoadStringA LoadStringA LoadStringA LoadStringA LoadStringA LoadStringA LoadStringA LoadStringA LoadStringA LoadStringA LoadStringA LoadStringA LoadStringA LoadStringA LoadStringA LoadStringA LoadStringA LoadStringA LoadStringA LoadStringA LoadStringA LoadStringA LoadStringA LoadStringA LoadStringA LoadStringA LoadStringA LoadStringA LoadStringA LoadStringA LoadStringA LoadStringA LoadStringA LdrGetDllHandle LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetDllHandle LdrGetProcedureAddress GetSystemMetrics GetSystemMetrics FindResourceA FindResourceA LoadResource SizeofResource NtAllocateVirtualMemory NtAllocateVirtualMemory LdrLoadDll LdrGetProcedureAddress LdrGetProcedureAddress GetSystemWindowsDirectoryW NtCreateFile NtCreateSection NtMapViewOfSection NtClose NtClose GetSystemMetrics NtAllocateVirtualMemory CreateActCtxW GetSystemWindowsDirectoryW CreateActCtxW LdrGetDllHandle LdrGetProcedureAddress LdrLoadDll LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrLoadDll LdrGetProcedureAddress GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics LdrGetProcedureAddress GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics FindResourceExW LoadResource GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics NtAllocateVirtualMemory LdrLoadDll LdrGetProcedureAddress LdrGetProcedureAddress LdrLoadDll NtQuerySystemInformation RegOpenKeyExA RegQueryValueExA RegCloseKey NtOpenKey NtQueryValueKey NtClose NtOpenKey NtQueryValueKey NtClose NtOpenKey NtQueryValueKey NtClose RegOpenKeyExW GlobalMemoryStatusEx NtOpenKey NtOpenKey NtQueryValueKey NtClose LdrGetProcedureAddress NtDuplicateObject LdrGetProcedureAddress LdrLoadDll LdrGetProcedureAddress NtCreateThreadEx NtDuplicateObject NtResumeThread LdrGetProcedureAddress LdrGetProcedureAddress NtClose NtOpenKey NtClose NtOpenKey NtQueryValueKey NtQueryValueKey NtClose RegOpenKeyExW RegQueryValueExW RegCloseKey LdrLoadDll NtOpenProcess NtClose NtCreateMutant LdrGetProcedureAddress GetSystemTimeAsFileTime GetSystemTimeAsFileTime GetSystemTimeAsFileTime GetSystemTimeAsFileTime GetSystemTimeAsFileTime GetSystemTimeAsFileTime GetSystemTimeAsFileTime GetSystemTimeAsFileTime GetSystemWindowsDirectoryW CreateProcessInternalW GetSystemTimeAsFileTime GetSystemTimeAsFileTime GetSystemTimeAsFileTime GetSystemTimeAsFileTime GetSystemTimeAsFileTime GetSystemTimeAsFileTime GetSystemTimeAsFileTime GetSystemTimeAsFileTime GetSystemTimeAsFileTime GetSystemTimeAsFileTime GetSystemTimeAsFileTime GetSystemTimeAsFileTime GetSystemTimeAsFileTime GetSystemTimeAsFileTime GetSystemTimeAsFileTime GetSystemTimeAsFileTime NtClose NtClose NtClose NtClose LdrUnloadDll LdrLoadDll NtOpenProcess NtClose NtCreateMutant NtClose NtClose LdrUnloadDll LdrLoadDll NtOpenProcess NtClose NtCreateMutant NtClose NtClose LdrUnloadDll FindResourceExW LoadResource FindResourceExW LoadResource FindResourceExW LoadResource FindResourceExW LoadResource FindResourceExW LoadResource FindResourceExW LoadResource FindResourceExW LoadResource FindResourceExW LoadResource FindResourceExW LoadResource FindResourceExW LoadResource FindResourceExW LoadResource FindResourceExW LoadResource FindResourceExW LoadResource FindResourceExW LoadResource FindResourceExW LoadResource FindResourceExW LoadResource FindResourceExW LoadResource FindResourceExW LoadResource FindResourceExW LoadResource FindResourceExW LoadResource FindResourceExW LoadResource FindResourceExW LoadResource FindResourceExW LoadResource FindResourceExW LoadResource LdrLoadDll LdrGetProcedureAddress NtClose NtOpenKey RegOpenKeyExW LdrLoadDll LdrGetProcedureAddress NtClose RegOpenKeyExW RegQueryValueExW RegCloseKey RegCloseKey LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrLoadDll NtOpenProcess NtClose NtCreateMutant NtClose NtClose LdrUnloadDll LdrLoadDll NtOpenProcess NtClose NtCreateMutant NtClose NtClose LdrUnloadDll LoadStringW FindResourceExW LoadResource EnumWindows GetSystemMetrics NtAllocateVirtualMemory GetSystemMetrics LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrLoadDll NtOpenProcess NtClose NtCreateMutant NtClose CreateThread NtClose NtClose NtClose LdrGetProcedureAddress LdrLoadDll LdrUnloadDll LdrGetProcedureAddress LdrLoadDll LdrUnloadDll LdrGetProcedureAddress LdrLoadDll LdrUnloadDll LdrGetProcedureAddress LdrLoadDll LdrUnloadDll GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics NtOpenSection NtMapViewOfSection RegOpenKeyExW RegQueryValueExW RegCloseKey RegOpenKeyExW LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrLoadDll LdrUnloadDll LdrLoadDll LdrUnloadDll LdrLoadDll LdrUnloadDll LdrLoadDll LdrUnloadDll LdrLoadDll LdrUnloadDll LoadStringW LoadStringW GetKeyState LdrLoadDll LdrUnloadDll LdrLoadDll LdrUnloadDll LdrLoadDll LdrUnloadDll LdrLoadDll LdrUnloadDll LdrLoadDll LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress GetNativeSystemInfo NtOpenProcess NtClose NtCreateSection LdrLoadDll LdrUnloadDll NtClose NtAllocateVirtualMemory LdrLoadDll LdrUnloadDll LdrLoadDll LdrUnloadDll DrawTextExW GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics DrawTextExW GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics DrawTextExW GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics DrawTextExW NtClose NtClose RegOpenKeyExW GetSystemDirectoryW LdrLoadDll LdrGetProcedureAddress LdrGetProcedureAddress CoInitializeEx LdrGetProcedureAddress LdrGetProcedureAddress NtClose NtClose RegOpenKeyExW RegQueryValueExW RegCloseKey NtClose NtClose NtClose NtClose NtClose NtClose GetSystemMetrics NtOpenMutant NtClose NtOpenMutant NtClose RegOpenKeyExW RegQueryValueExW RegCloseKey LdrGetDllHandle FindResourceExW FindResourceExW RegOpenKeyExW DrawTextExW GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics DrawTextExW DrawTextExW GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics DrawTextExW RegOpenKeyExW GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics LdrLoadDll LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress GetFileVersionInfoSizeW GetFileVersionInfoW DrawTextExW GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics DrawTextExW GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics DrawTextExW GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics DrawTextExW GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics DrawTextExW GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics DrawTextExW GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics DrawTextExW GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics DrawTextExW GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics DrawTextExW GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics DrawTextExW GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics DrawTextExW GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics DrawTextExW GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics DrawTextExW GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics DrawTextExW GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics DrawTextExW GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics DrawTextExW GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics DrawTextExW GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics DrawTextExW GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics DrawTextExW GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics DrawTextExW GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics DrawTextExW GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics DrawTextExW GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics DrawTextExW GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics DrawTextExW GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics DrawTextExW DrawTextExW GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics DrawTextExW GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics DrawTextExW DrawTextExW DrawTextExW GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics DrawTextExW GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics DrawTextExW DrawTextExW DrawTextExW DrawTextExW GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics DrawTextExW GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics DrawTextExW DrawTextExW DrawTextExW DrawTextExW DrawTextExW GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics DrawTextExW GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics NtAllocateVirtualMemory DrawTextExW DrawTextExW DrawTextExW DrawTextExW DrawTextExW DrawTextExW GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics DrawTextExW GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics FindResourceA FindResourceA LoadResource SizeofResource NtFreeVirtualMemory NtFreeVirtualMemory DrawTextExA GetCursorPos GetCursorPos GetSystemMetrics FindResourceExW FindResourceExW GetSystemMetrics GetSystemMetrics DrawTextExW GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics DrawTextExW GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics DrawTextExW GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics DrawTextExW GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics FindResourceExW LoadResource DrawTextExW GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics DrawTextExW GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics DrawTextExW GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics DrawTextExW GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics DrawTextExW GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics DrawTextExW GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics DrawTextExW GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics DrawTextExW GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics DrawTextExW DrawTextExW GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics DrawTextExW GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics DrawTextExW GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics DrawTextExW GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics DrawTextExW GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics DrawTextExW GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics DrawTextExW GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics DrawTextExW GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics DrawTextExA GetCursorPos NtCreateFile NtQueryInformationFile NtAllocateVirtualMemory NtAllocateVirtualMemory NtReadFile NtWriteFile NtSetInformationFile NtFreeVirtualMemory NtClose NtCreateFile NtQueryInformationFile NtAllocateVirtualMemory NtAllocateVirtualMemory NtReadFile NtWriteFile NtSetInformationFile NtFreeVirtualMemory NtClose NtCreateFile NtQueryInformationFile NtAllocateVirtualMemory NtAllocateVirtualMemory NtReadFile NtWriteFile NtSetInformationFile NtFreeVirtualMemory NtClose NtCreateFile NtQueryInformationFile NtAllocateVirtualMemory NtAllocateVirtualMemory NtReadFile NtWriteFile NtSetInformationFile NtFreeVirtualMemory NtClose NtCreateFile NtQueryInformationFile NtAllocateVirtualMemory NtAllocateVirtualMemory NtReadFile NtWriteFile NtSetInformationFile NtFreeVirtualMemory NtClose __exception__ FindResourceA FindResourceA SizeofResource LoadResource NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtFreeVirtualMemory NtFreeVirtualMemory NtFreeVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtDuplicateObject NtClose NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtua</t>
-  </si>
-  <si>
-    <t>192.168.56.101:49360 192.168.56.101:55311 192.168.56.101:137 192.168.56.101:64412 192.168.56.101:58084 192.168.56.101:54425 192.168.56.101:52057 192.168.56.101:59469 192.168.56.101:54227 192.168.56.101:123 192.168.56.101:1900</t>
-  </si>
-  <si>
-    <t>224.0.0.252:5355 239.255.255.250:1900 192.168.56.255:137 224.0.0.252:5355 224.0.0.252:5355 8.8.8.8:53 224.0.0.252:5355 224.0.0.252:5355 8.8.8.8:53 13.65.88.161:123 239.255.255.250:1900</t>
-  </si>
-  <si>
-    <t>softcnapp</t>
-  </si>
-  <si>
-    <t>0271c5b2484ec857619b56cbeaa5e438</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GetSystemTimeAsFileTime LdrLoadDll LdrLoadDll LdrGetProcedureAddress LdrLoadDll LdrGetProcedureAddress LdrGetProcedureAddress LdrLoadDll LdrGetProcedureAddress LdrGetProcedureAddress LdrLoadDll LdrLoadDll LdrGetProcedureAddress LdrLoadDll LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrLoadDll LdrGetProcedureAddress LdrGetDllHandle LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetDllHandle LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress SetUnhandledExceptionFilter LdrLoadDll LdrGetProcedureAddress LdrGetProcedureAddress NtOpenKey NtQueryValueKey NtClose NtOpenKey NtQueryValueKey NtClose NtOpenKey NtQueryValueKey NtClose NtOpenKey NtQueryValueKey NtClose LdrGetProcedureAddress NtClose NtOpenKey NtQueryValueKey NtClose NtOpenKey NtQueryValueKey NtClose NtOpenKey NtQueryValueKey NtClose NtOpenKey NtQueryValueKey NtClose NtOpenKey NtQueryValueKey NtClose NtOpenKey NtQueryValueKey NtClose NtOpenKey NtQueryValueKey NtClose NtOpenKey NtQueryValueKey NtClose NtOpenKey NtQueryValueKey NtClose NtOpenKey NtQueryValueKey NtClose NtOpenKey NtQueryValueKey NtClose NtOpenKey NtQueryValueKey NtClose NtOpenKey NtQueryValueKey NtClose NtOpenKey NtQueryValueKey NtClose NtOpenKey NtQueryValueKey GetFileAttributesW SHGetFolderPathW SHGetFolderPathW SetErrorMode GetFileAttributesW SetErrorMode SetErrorMode GetFileAttributesW SetErrorMode SetErrorMode GetFileAttributesW SetErrorMode SetErrorMode GetFileAttributesW SetErrorMode NtAllocateVirtualMemory SetErrorMode GetFileAttributesW SetErrorMode SetErrorMode GetFileAttributesW SetErrorMode SetErrorMode GetFileAttributesW SetErrorMode SetErrorMode GetFileAttributesW SetErrorMode SetErrorMode GetFileAttributesW SetErrorMode SetErrorMode GetFileAttributesW SetErrorMode CreateDirectoryW LdrLoadDll GetSystemTimeAsFileTime GetTimeZoneInformation NtCreateFile DeviceIoControl DeviceIoControl NtClose NtCreateFile NtCreateFile NtCreateFile NtCreateFile NtCreateFile NtCreateFile NtCreateFile NtCreateFile NtCreateFile NtCreateFile NtCreateFile NtCreateFile NtCreateFile NtCreateFile NtCreateFile GetAdaptersInfo GetAdaptersInfo GetSystemDirectoryW NtOpenFile NtQueryInformationFile NtClose CoInitializeEx WSAStartup GetSystemTimeAsFileTime LdrLoadDll GetSystemTimeAsFileTime LdrLoadDll CoCreateInstance NtClose NtClose GetSystemMetrics NtAllocateVirtualMemory GetSystemMetrics GetSystemMetrics LdrLoadDll LdrGetProcedureAddress GetSystemMetrics GetSystemMetrics NtClose NtClose RegOpenKeyExW GetSystemDirectoryW LdrLoadDll LdrGetProcedureAddress LdrGetProcedureAddress CoInitializeEx LdrGetProcedureAddress LdrGetProcedureAddress NtClose NtClose RegOpenKeyExW RegQueryValueExW RegCloseKey NtClose NtClose NtClose NtClose NtClose NtClose GetSystemMetrics NtOpenMutant NtClose NtOpenMutant NtClose NtAllocateVirtualMemory NtAllocateVirtualMemory RegOpenKeyExW RegQueryValueExW RegCloseKey RegOpenKeyExW NtAllocateVirtualMemory LdrGetDllHandle FindResourceExW FindResourceExW LdrLoadDll LdrLoadDll FindResourceW LoadResource SizeofResource NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtFreeVirtualMemory NtAllocateVirtualMemory GetSystemInfo LdrGetDllHandle LdrGetProcedureAddress LdrGetDllHandle LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress GetSystemMetrics GetSystemMetrics GetSystemMetrics LdrGetDllHandle LdrGetProcedureAddress LdrGetProcedureAddress GetSystemDirectoryW LdrLoadDll CreateThread GetSystemMetrics GetSystemMetrics FindResourceExW LoadResource FindResourceExW LoadResource LdrGetDllHandle GetSystemMetrics GetSystemMetrics FindResourceExW LoadResource FindResourceExW LoadResource NtFreeVirtualMemory NtFreeVirtualMemory NtFreeVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtFreeVirtualMemory NtAllocateVirtualMemory NtFreeVirtualMemory NtAllocateVirtualMemory NtFreeVirtualMemory NtFreeVirtualMemory NtFreeVirtualMemory NtFreeVirtualMemory NtFreeVirtualMemory NtFreeVirtualMemory LdrGetDllHandle LdrGetProcedureAddress CoCreateInstance NtAllocateVirtualMemory GetSystemMetrics GetSystemMetrics NtAllocateVirtualMemory FindResourceExW NtClose NtClose RegOpenKeyExW LdrLoadDll LdrLoadDll FindResourceW LoadResource SizeofResource NtAllocateVirtualMemory NtAllocateVirtualMemory GetSystemMetrics GetSystemMetrics FindResourceExW LoadResource FindResourceExW LoadResource LdrGetDllHandle GetSystemMetrics GetSystemMetrics FindResourceExW LoadResource FindResourceExW LoadResource CreateToolhelp32Snapshot Process32FirstW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW NtClose CreateToolhelp32Snapshot Process32FirstW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW NtClose CreateToolhelp32Snapshot Process32FirstW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW NtClose CreateToolhelp32Snapshot Process32FirstW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW NtClose CreateToolhelp32Snapshot Process32FirstW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW NtClose CreateToolhelp32Snapshot Process32FirstW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW NtClose CreateToolhelp32Snapshot Process32FirstW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW NtClose CreateToolhelp32Snapshot Process32FirstW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW NtClose CreateToolhelp32Snapshot Process32FirstW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW NtClose CreateToolhelp32Snapshot Process32FirstW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW NtClose NtFreeVirtualMemory NtFreeVirtualMemory NtFreeVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory CoCreateInstance SetWindowsHookExW SetWindowsHookExW NtOpenSection NtMapViewOfSection LdrLoadDll LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetDllHandle LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress RegOpenKeyExW RegQueryValueExW RegOpenKeyExW RegQueryValueExW RegOpenKeyExW RegQueryValueExW RegOpenKeyExW RegQueryValueExW LdrGetDllHandle LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegQueryValueExW RegQueryValueExW RegOpenKeyExW RegQueryValueExW RegCloseKey RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegCloseKey RegCloseKey RegCloseKey RegCloseKey RegOpenKeyExW RegQueryValueExW RegOpenKeyExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW NtClose RegOpenKeyExW RegOpenKeyExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegOpenKeyExW RegQueryValueExW RegCloseKey LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress RegOpenKeyExW RegQueryValueExW RegCloseKey RegOpenKeyExW RegOpenKeyExW RegQueryValueExW RegCloseKey RegOpenKeyExW RegOpenKeyExW RegQueryValueExW RegCloseKey RegOpenKeyExW RegOpenKeyExW RegQueryValueExW RegCloseKey RegOpenKeyExW RegOpenKeyExW RegQueryValueExW RegCloseKey RegOpenKeyExW RegOpenKeyExA LdrGetProcedureAddress LdrGetProcedureAddress LdrLoadDll LdrGetProcedureAddress RegOpenKeyExW RegQueryValueExW RegCloseKey RegOpenKeyExW RegOpenKeyExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegCloseKey RegOpenKeyExW RegQueryValueExW RegCloseKey RegOpenKeyExW RegOpenKeyExW RegQueryValueExW RegCloseKey RegOpenKeyExW RegQueryValueExW RegQueryValueExW RegCloseKey RegOpenKeyExW RegOpenKeyExW NtOpenKey NtQueryValueKey NtClose LdrGetDllHandle RegOpenKeyExW RegCloseKey RegOpenKeyExW RegQueryValueExW RegCloseKey NtOpenKey NtOpenKey NtQueryValueKey NtClose CoCreateInstance RegOpenKeyExA RegOpenKeyExW RegQueryValueExW RegCloseKey RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegCloseKey RegCloseKey RegCloseKey RegCloseKey RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegQueryValueExW RegCloseKey RegOpenKeyExW FindResourceExW LoadResource FindResourceExW LoadResource FindResourceExW LoadResource FindResourceExW LoadResource FindResourceExW LoadResource FindResourceExW LoadResource FindResourceExW LoadResource FindResourceExW LoadResource FindResourceExW LoadResource FindResourceExW LoadResource FindResourceExW LoadResource FindResourceExW LoadResource FindResourceExW LoadResource FindResourceExW LoadResource FindResourceExW LoadResource FindResourceExW LoadResource FindResourceExW LoadResource FindResourceExW LoadResource FindResourceExW LoadResource FindResourceExW LoadResource FindResourceExW LoadResource FindResourceExW LoadResource FindResourceExW LoadResource FindResourceExW LoadResource FindResourceExW LoadResource FindResourceExW LoadResource FindResourceExW LoadResource FindResourceExW LoadResource FindResourceExW LoadResource FindResourceExW LoadResource FindResourceExW LoadResource FindResourceExW LoadResource FindResourceExW LoadResource FindResourceExW LoadResource FindResourceExW LoadResource FindResourceExW LoadResource FindResourceExW LoadResource CoInitializeEx CoUninitialize LdrGetProcedureAddress RegOpenKeyExA RegOpenKeyExA RegOpenKeyExA RegCloseKey RegOpenKeyExW RegOpenKeyExW RegQueryValueExA RegCloseKey NtOpenSection NtQueryAttributesFile NtQueryAttributesFile NtOpenFile NtCreateSection NtMapViewOfSection NtClose NtClose NtProtectVirtualMemory NtOpenSection NtMapViewOfSection NtClose NtProtectVirtualMemory NtProtectVirtualMemory NtProtectVirtualMemory GetSystemTimeAsFileTime GetSystemTimeAsFileTime RegOpenKeyExW RegQueryValueExW RegCloseKey RegOpenKeyExW RegQueryValueExW RegCloseKey RegOpenKeyExW RegQueryValueExW RegCloseKey CoGetClassObject LdrGetProcedureAddress LdrGetProcedureAddress RegOpenKeyExW RegOpenKeyExA RegEnumValueA RegEnumValueA RegEnumValueA RegEnumValueA RegEnumValueA RegEnumValueA RegEnumValueA RegEnumValueA RegEnumValueA RegEnumValueA RegEnumValueA RegEnumValueA RegEnumValueA LdrGetProcedureAddress RegCloseKey RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegQueryValueExA RegCloseKey CoGetClassObject RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegCloseKey RegCloseKey RegCloseKey RegCloseKey LdrGetProcedureAddress RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegQueryInfoKeyW RegCloseKey RegOpenKeyExW RegQueryInfoKeyW RegCloseKey RegOpenKeyExW RegQueryValueExW RegCloseKey LdrGetProcedureAddress RegOpenKeyExW RegQueryValueExW RegCloseKey RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegCloseKey RegCloseKey RegCloseKey RegCloseKey RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegQueryValueExW RegQueryValueExW NtCreateMutant RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegCloseKey RegCloseKey RegCloseKey RegCloseKey RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegQueryInfoKeyW RegCloseKey RegOpenKeyExW RegQueryInfoKeyW RegEnumValueW RegEnumValueW RegEnumValueW RegEnumValueW RegEnumValueW RegEnumValueW RegEnumValueW RegCloseKey RegOpenKeyExW RegQueryInfoKeyW RegCloseKey RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegQueryValueExW RegCloseKey RegOpenKeyExW RegQueryValueExW RegCloseKey GetUserNameW NtCreateSection NtMapViewOfSection NtCreateMutant RegOpenKeyExW RegQueryValueExW RegCloseKey RegOpenKeyExW RegOpenKeyExW RegCloseKey RegOpenKeyExW RegCloseKey RegOpenKeyExW RegCloseKey RegOpenKeyExW RegCloseKey RegOpenKeyExW RegCloseKey RegCloseKey RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegEnumKeyExW NtCreateMutant RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegQueryValueExW RegCloseKey RegCloseKey RegEnumKeyExW RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegQueryValueExW RegOpenKeyExW RegDeleteValueW RegOpenKeyExW RegDeleteValueW RegDeleteValueW RegDeleteValueW RegSetValueExW RegSetValueExW RegCloseKey RegCloseKey RegCloseKey RegCloseKey RegEnumKeyExW RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegQueryValueExW RegCloseKey RegCloseKey RegEnumKeyExW RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegQueryValueExW RegCloseKey RegCloseKey RegEnumKeyExW RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegQueryValueExW RegCloseKey RegCloseKey RegEnumKeyExW RegCloseKey RegOpenKeyExW RegQueryValueExW RegQueryValueExW RegOpenKeyExW RegQueryValueExW RegQueryValueExW NtCreateMutant RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegEnumKeyExW NtCreateMutant RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegQueryValueExW RegCloseKey RegCloseKey RegEnumKeyExW RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegQueryValueExW RegOpenKeyExW RegDeleteValueW RegOpenKeyExW RegDeleteValueW RegDeleteValueW RegDeleteValueW RegSetValueExW RegSetValueExW RegCloseKey RegCloseKey RegCloseKey RegCloseKey RegEnumKeyExW RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegQueryValueExW RegCloseKey RegCloseKey RegEnumKeyExW RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegQueryValueExW RegCloseKey RegCloseKey RegEnumKeyExW RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegQueryValueExW RegCloseKey RegCloseKey RegEnumKeyExW RegCloseKey RegOpenKeyExW RegOpenKeyExW RegQueryValueExA RegCloseKey CoGetClassObject RegOpenKeyExW RegOpenKeyExW RegQueryValueExA RegCloseKey CoGetClassObject RegCloseKey RegCloseKey RegOpenKeyExW RegQueryValueExW RegOpenKeyExW RegQueryValueExW RegOpenKeyExW RegQueryValueExW RegOpenKeyExW RegQueryValueExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegOpenKeyExW RegOpenKeyExW RegQueryValueExA RegCloseKey CoGetClassObject RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegQueryValueExW RegOpenKeyExW RegOpenKeyExW RegQueryValueExA RegCloseKey CoGetClassObject GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics RegCloseKey GetSystemWindowsDirectoryW CreateActCtxW LdrLoadDll LdrGetDllHandle LdrLoadDll LdrGetProcedureAddress LdrGetProcedureAddress NtUnmapViewOfSection NtClose RegOpenKeyExW RegQueryValueExW RegCloseKey RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegQueryValueExW RegQueryValueExW RegCloseKey RegCloseKey RegCloseKey RegCloseKey RegCloseKey RegOpenKeyExW RegOpenKeyExW RegQueryValueExA RegCloseKey CoGetClassObject RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegQueryValueExW RegOpenKeyExA RegQueryValueExA RegCloseKey RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegQueryValueExW RegOpenKeyExW RegQueryValueExW RegCloseKey RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegCloseKey RegCloseKey RegCloseKey RegCloseKey RegOpenKeyExW RegCloseKey RegOpenKeyExW RegQueryValueExW RegCloseKey LoadStringW RegOpenKeyExW RegQueryValueExW RegCloseKey LoadStringW RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegQueryValueExW CoGetClassObject GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics RegCloseKey GetSystemWindowsDirectoryW CreateActCtxW NtClose NtOpenKey NtClose NtOpenKey NtQueryValueKey NtClose NtClose NtOpenKey NtClose NtOpenKey NtQueryValueKey NtClose NtClose NtOpenKey NtClose NtOpenKey NtQueryValueKey NtClose NtClose NtOpenKey NtClose NtOpenKey NtQueryValueKey NtClose ReadProcessMemory ReadProcessMemory ReadProcessMemory ReadProcessMemory ReadProcessMemory RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegCloseKey RegCloseKey RegCloseKey RegCloseKey RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegQueryValueExW RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegQueryValueExW RegCloseKey RegOpenKeyExW RegQueryValueExW RegCloseKey RegOpenKeyExW RegOpenKeyExW RegQueryValueExA RegCloseKey CoGetClassObject RegOpenKeyExW RegOpenKeyExW RegQueryValueExA RegCloseKey CoGetClassObject RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegCloseKey RegCloseKey RegCloseKey RegCloseKey RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegQueryValueExW RegOpenKeyExW RegQueryValueExW RegCloseKey RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegCloseKey RegCloseKey RegCloseKey RegCloseKey LdrGetDllHandle LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress RegOpenKeyExW RegOpenKeyExW RegQueryValueExA RegCloseKey CoGetClassObject RegOpenKeyExW RegQueryValueExW RegOpenKeyExA RegOpenKeyExA RegOpenKeyExA RegCloseKey RegOpenKeyExW RegOpenKeyExW RegQueryValueExA RegCloseKey CoGetClassObject RegCloseKey RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegCloseKey RegCloseKey RegCloseKey RegCloseKey RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegQueryValueExW RegCloseKey RegOpenKeyExW RegQueryValueExW RegCloseKey RegCloseKey RegCloseKey RegOpenKeyExW RegCloseKey RegQueryValueExW RegQueryValueExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegOpenKeyExW RegOpenKeyExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegQueryValueExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegOpenKeyExW RegQueryValueExW RegOpenKeyExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegQueryValueExW RegQueryValueExW RegOpenKeyExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW LdrGetDllHandle LdrGetDllHandle LdrGetDllHandle LdrGetDllHandle RegOpenKeyExW RegQueryValueExW RegCloseKey RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegOpenKeyExA RegQueryValueExW RegCloseKey RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegCloseKey RegQueryInfoKeyW RegEnumValueW RegEnumValueW RegEnumValueW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegOpenKeyExW RegOpenKeyExW RegQueryValueExA RegCloseKey CoGetClassObject RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegQueryValueExW LdrGetProcedureAddress LdrGetProcedureAddress RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegQueryValueExW RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegQueryValueExW RegQueryValueExW RegCloseKey RegCloseKey RegCloseKey RegCloseKey RegCloseKey GetCursorPos GetKeyState GetKeyState GetKeyState GetKeyState GetKeyState GetKeyState LdrGetProcedureAddress RegOpenKeyExW RegQueryValueExW RegCloseKey NtAllocateVirtualMemory NtAllocateVirtualMemory LdrLoadDll LdrGetProcedureAddress LdrGetProcedureAddress RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegQueryValueExW RegQueryValueExW RegCloseKey RegCloseKey RegCloseKey RegCloseKey RegCloseKey RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegCloseKey RegCloseKey RegCloseKey RegCloseKey FindWindowW FindWindowW NtAllocateVirtualMemory CreateThread LdrGetProcedureAddress RegOpenKeyExW RegQueryValueExW RegCloseKey NtAllocateVirtualMemory RegOpenKeyExW RegQueryValueExW RegCloseKey RegOpenKeyExW RegOpenKeyExW RegQueryValueExW RegCloseKey LdrGetProcedureAddress RegOpenKeyExW RegQueryValueExW RegCloseKey RegOpenKeyExW RegQueryValueExW RegCloseKey NtAllocateVirtualMemory RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegCloseKey RegCloseKey RegCloseKey RegCloseKey LdrLoadDll CoInitializeEx LoadStringW LoadStringW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegCloseKey RegCloseKey RegOpenKeyExW RegOpenKeyExW LoadStringW LoadStringW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegCloseKey RegCloseKey RegOpenKeyExW RegQueryValueExW RegCloseKey RegOpenKeyExW RegQueryValueExW RegCloseKey RegOpenKeyExW RegOpenKeyExW LoadStringW LoadStringW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegCloseKey RegCloseKey RegOpenKeyExW RegQueryValueExW RegOpenKeyExW RegQueryValueExW RegCloseKey RegCloseKey RegOpenKeyExW RegQueryValueExW RegCloseKey RegOpenKeyExW RegOpenKeyExW LoadStringW LoadStringW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegCloseKey RegCloseKey RegOpenKeyExW RegQueryValueExW RegOpenKeyExW RegQueryValueExW RegCloseKey RegCloseKey RegOpenKeyExW RegQueryValueExW RegCloseKey RegOpenKeyExW RegOpenKeyExW LoadStringW LoadStringW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegCloseKey RegCloseKey RegOpenKeyExW RegQueryValueExW RegOpenKeyExW RegQueryValueExW RegCloseKey RegCloseKey RegOpenKeyExW RegQueryValueExW RegCloseKey LdrGetProcedureAddress RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegCloseKey RegCloseKey RegCloseKey RegCloseKey NtOpenMutant NtClose NtClose NtClose NtCreateMutant NtDuplicateObject NtClose RegOpenKeyExW RegCloseKey RegQueryValueExW RegQueryValueExW LdrLoadDll LdrGetProcedureAddress GetFileVersionInfoSizeW LdrGetProcedureAddress GetFileVersionInfoW LdrGetProcedureAddress NtClose RegQueryValueExW RegQueryValueExW GetUserNameA NtClose RegCreateKeyExA RegQueryValueExA LdrGetDllHandle LdrGetProcedureAddress RegOpenKeyExA RegQueryValueExA RegCloseKey RegOpenKeyExA RegOpenKeyExA RegOpenKeyExA RegQueryValueExA RegCloseKey RegOpenKeyExA RegQueryValueExA RegOpenKeyExA RegQueryValueExA RegCloseKey RegCloseKey RegOpenKeyExA LdrLoadDll LdrGetProcedureAddress SHGetFolderPathW GetFileAttributesW GetFileAttributesW GetFileAttributesW GetFileAttributesW GetFileAttributesW GetFileAttributesW RegQueryValueExA RegQueryValueExA RegOpenKeyExA RegQueryValueExA RegOpenKeyExA RegQueryValueExA RegCloseKey RegCloseKey RegCloseKey RegOpenKeyExA SHGetFolderPathW GetFileAttributesW RegQueryValueExA RegQueryValueExA RegOpenKeyExA RegQueryValueExA RegOpenKeyExA RegQueryValueExA RegCloseKey RegCloseKey RegCloseKey RegOpenKeyExA SHGetFolderPathW GetFileAttributesW GetFileAttributesW GetFileAttributesW GetFileAttributesW GetFileAttributesW GetFileAttributesW RegQueryValueExA RegQueryValueExA RegCloseKey RegCloseKey RegCloseKey NtOpenMutant NtOpenMutant GetFileAttributesW SetFileAttributesW NtCreateFile GetFileAttributesW SetFileTime GetFileSize NtOpenSection NtMapViewOfSection NtOpenMutant GetFileAttributesW SetFileAttributesW NtCreateFile GetFileAttributesW SetFileTime GetFileSize NtOpenSection NtMapViewOfSection NtOpenMutant GetFileAttributesW SetFileAttributesW NtCreateFile GetFileAttributesW SetFileTime GetFileSize NtOpenSection NtMapViewOfSection GetFileAttributesW GetFileAttributesW GetFileAttributesW GetFileAttributesW RegOpenKeyExA RegOpenKeyExA RegCloseKey RegEnumKeyExA RegOpenKeyExA RegQueryValueExA RegQueryValueExA RegQueryValueExA RegQueryValueExA RegQueryValueExA RegCloseKey RegEnumKeyExA RegOpenKeyExA RegQueryValueExA RegQueryValueExA RegQueryValueExA RegQueryValueExA RegQueryValueExA RegCloseKey RegEnumKeyExA RegOpenKeyExA RegQueryValueExA RegQueryValueExA RegQueryValueExA RegQueryValueExA RegQueryValueExA RegCloseKey RegEnumKeyExA RegOpenKeyExA RegQueryValueExA RegQueryValueExA RegQueryValueExA RegQueryValueExA RegQueryValueExA NtAllocateVirtualMemory RegCloseKey RegEnumKeyExA RegOpenKeyExA RegQueryValueExA RegQueryValueExA RegQueryValueExA RegQueryValueExA RegQueryValueExA RegCloseKey RegEnumKeyExA RegCloseKey NtOpenMutant NtCreateMutant GetFileAttributesW SetFileAttributesW NtCreateFile GetFileAttributesW SetFileTime GetFileSize NtOpenSection NtCreateSection NtMapViewOfSection RegOpenKeyExW RegQueryValueExW RegCloseKey NtAllocateVirtualMemory NtAllocateVirtualMemory CreateThread RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegQueryValueExW RegQueryValueExW RegCloseKey RegCloseKey RegCloseKey RegCloseKey </t>
-  </si>
-  <si>
-    <t>192.168.56.101:49360 192.168.56.101:50300 192.168.56.101:64412 192.168.56.101:137 192.168.56.101:1900 192.168.56.101:53352 192.168.56.101:64413 192.168.56.101:138 192.168.56.101:64415 192.168.56.101:58084 192.168.56.101:54425 192.168.56.101:52057 192.168.56.101:59469 192.168.56.101:54227 192.168.56.101:54228 192.168.56.101:54230 192.168.56.101:52887 192.168.56.101:63529 192.168.56.101:51765 192.168.56.101:49465 192.168.56.101:50974 192.168.56.101:55167 192.168.56.101:63794 192.168.56.101:62948 192.168.56.101:49746</t>
-  </si>
-  <si>
-    <t>8.8.8.8:53 239.255.255.250:3702 224.0.0.252:5355 192.168.56.255:137 239.255.255.250:1900 239.255.255.250:1900 239.255.255.250:3702 192.168.56.255:138 239.255.255.250:3702 224.0.0.252:5355 8.8.8.8:53 224.0.0.252:5355 224.0.0.252:5355 224.0.0.252:5355 239.255.255.250:3702 239.255.255.250:3702 224.0.0.252:5355 224.0.0.252:5355 224.0.0.252:5355 8.8.8.8:53 224.0.0.252:5355 8.8.8.8:53 8.8.8.8:53 224.0.0.252:5355 8.8.8.8:53</t>
+    <t>chisburg</t>
+  </si>
+  <si>
+    <t>01937e210ea0db9d997ce6c4284e1977</t>
+  </si>
+  <si>
+    <t>RegOpenKeyExA RegOpenKeyExA RegOpenKeyExA NtOpenKey NtQueryValueKey NtClose NtOpenKey NtQueryValueKey NtClose NtClose NtQueryAttributesFile NtQueryAttributesFile NtQueryAttributesFile NtQueryAttributesFile LoadStringA NtAllocateVirtualMemory NtAllocateVirtualMemory LoadStringA LoadStringA LoadStringA LoadStringA LoadStringA LoadStringA LoadStringA LoadStringA LoadStringA LoadStringA LoadStringA LoadStringA LoadStringA LoadStringA LoadStringA LoadStringA LoadStringA LoadStringA LoadStringA LoadStringA LoadStringA LoadStringA LoadStringA LoadStringA LoadStringA LoadStringA LoadStringA LoadStringA LoadStringA LoadStringA LdrGetDllHandle LdrGetProcedureAddress LdrGetDllHandle LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetDllHandle LoadStringA LoadStringA LoadStringA LoadStringA LoadStringA LoadStringA LoadStringA LoadStringA LoadStringA LoadStringA LoadStringA LoadStringA LoadStringA LoadStringA LoadStringA LoadStringA LoadStringA LoadStringA LoadStringA LoadStringA LoadStringA LoadStringA LoadStringA LoadStringA LoadStringA LoadStringA LoadStringA LoadStringA LoadStringA LoadStringA LoadStringA LoadStringA LoadStringA LoadStringA LoadStringA LoadStringA LoadStringA LoadStringA LoadStringA LoadStringA LoadStringA LoadStringA LoadStringA LoadStringA LoadStringA LoadStringA LoadStringA LoadStringA LoadStringA LoadStringA LoadStringA LoadStringA LoadStringA LoadStringA LoadStringA LoadStringA LoadStringA LoadStringA LoadStringA LoadStringA LoadStringA LoadStringA LoadStringA LoadStringA LoadStringA LdrGetProcedureAddress LdrGetProcedureAddress GetSystemMetrics GetSystemMetrics FindResourceExW LoadResource FindResourceExW LoadResource FindResourceExW LoadResource FindResourceExW LoadResource FindResourceExW LoadResource FindResourceExW LoadResource FindResourceExW LoadResource FindResourceExW LoadResource FindResourceExW LoadResource FindResourceExW LoadResource FindResourceExW LoadResource FindResourceExW LoadResource FindResourceExW LoadResource FindResourceExW LoadResource LdrGetProcedureAddress FindResourceExW LoadResource FindResourceExW LoadResource NtAllocateVirtualMemory GetSystemMetrics GetSystemMetrics NtClose NtClose GetSystemMetrics NtAllocateVirtualMemory GetSystemMetrics GetSystemMetrics LdrLoadDll LdrGetProcedureAddress LdrGetDllHandle FindResourceExW LoadResource FindResourceExW LoadResource DrawTextExW GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics GetSystemMetrics DrawTextExW LdrGetDllHandle FindResourceExW LoadResource FindResourceExW LoadResource FindResourceExW LoadResource LdrGetDllHandle LdrGetProcedureAddress LdrGetDllHandle LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetDllHandle LdrGetProcedureAddress FindResourceExW LoadResource FindResourceExW LoadResource LoadStringA LoadStringA LoadStringA LoadStringA LoadStringA LoadStringA LoadStringA LoadStringA LoadStringA LoadStringA LoadStringA LoadStringA LoadStringA LoadStringA GetTempPathW LoadStringA LoadStringA LoadStringA LoadStringA LoadStringA LoadStringA LoadStringA LoadStringA LoadStringA NtAllocateVirtualMemory NtFreeVirtualMemory LdrGetDllHandle LdrGetDllHandle LdrGetProcedureAddress NtDelayExecution NtDelayExecution NtDelayExecution NtDelayExecution NtDelayExecution NtDelayExecution NtDelayExecution NtDelayExecution NtDelayExecution NtDelayExecution NtDelayExecution NtDelayExecution NtDelayExecution NtDelayExecution NtDelayExecution NtDelayExecution NtDelayExecution NtDelayExecution NtDelayExecution NtDelayExecution NtDelayExecution NtDelayExecution NtDelayExecution NtDelayExecution NtDelayExecution NtDelayExecution NtDelayExecution NtDelayExecution NtDelayExecution NtAllocateVirtualMemory NtFreeVirtualMemory NtProtectVirtualMemory NtAllocateVirtualMemory LdrLoadDll LdrLoadDll LdrLoadDll NtAllocateVirtualMemory NtAllocateVirtualMemory NtFreeVirtualMemory NtAllocateVirtualMemory CreateToolhelp32Snapshot Process32FirstW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW Process32NextW NtTerminateProcess NtTerminateProcess NtClose NtClose NtClose NtClose NtClose NtClose NtClose NtClose NtClose NtClose NtClose NtClose NtClose NtClose LdrGetDllHandle LdrGetProcedureAddress LdrGetDllHandle LdrGetProcedureAddress NtClose LdrUnloadDll NtOpenKey NtQueryValueKey NtClose NtClose NtClose NtClose NtTerminateProcess</t>
+  </si>
+  <si>
+    <t>192.168.56.101:49360 192.168.56.101:64412 192.168.56.101:58084 192.168.56.101:54425 192.168.56.101:52057 192.168.56.101:59469 192.168.56.101:54227 192.168.56.101:50300 192.168.56.101:137 192.168.56.101:1900 192.168.56.101:54229 192.168.56.101:52887 192.168.56.101:63529 192.168.56.101:51765 192.168.56.101:138 192.168.56.101:49465 192.168.56.101:49466</t>
+  </si>
+  <si>
+    <t>224.0.0.252:5355 224.0.0.252:5355 224.0.0.252:5355 224.0.0.252:5355 224.0.0.252:5355 224.0.0.252:5355 8.8.8.8:53 239.255.255.250:3702 192.168.56.255:137 239.255.255.250:1900 239.255.255.250:1900 224.0.0.252:5355 224.0.0.252:5355 224.0.0.252:5355 192.168.56.255:138 8.8.8.8:53 239.255.255.250:3702</t>
+  </si>
+  <si>
+    <t>playtech</t>
+  </si>
+  <si>
+    <t>01c10152a298f9f44eae112cce55ca42</t>
+  </si>
+  <si>
+    <t>SetErrorMode OleInitialize LdrGetDllHandle LdrGetDllHandle LdrLoadDll LdrGetProcedureAddress LdrLoadDll LdrGetProcedureAddress LdrLoadDll LdrGetProcedureAddress LdrGetProcedureAddress NtOpenSection NtMapViewOfSection RegOpenKeyExW RegQueryValueExW RegCloseKey RegOpenKeyExW RegOpenKeyExW RegQueryValueExW RegCloseKey RegOpenKeyExW RegOpenKeyExW RegQueryValueExW RegCloseKey RegOpenKeyExW RegOpenKeyExW RegQueryValueExW RegCloseKey RegOpenKeyExW RegOpenKeyExW RegQueryValueExW RegCloseKey RegOpenKeyExW NtClose NtOpenKey NtQueryValueKey NtClose NtOpenKey NtQueryValueKey NtClose LdrLoadDll LdrGetProcedureAddress LdrGetProcedureAddress GetSystemWindowsDirectoryW NtCreateFile NtCreateSection NtMapViewOfSection NtClose NtClose RegOpenKeyExA LdrGetProcedureAddress CreateActCtxW LdrLoadDll LdrLoadDll LdrGetProcedureAddress GetSystemDirectoryW RegOpenKeyExA RegOpenKeyExA LdrLoadDll LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress RegOpenKeyExW RegQueryValueExW RegCloseKey RegOpenKeyExW LdrGetProcedureAddress LdrGetProcedureAddress RegOpenKeyExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegCloseKey LdrGetProcedureAddress RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegQueryValueExW RegCloseKey LdrGetProcedureAddress LdrGetProcedureAddress GetVolumeNameForVolumeMountPointW LdrGetProcedureAddress RegOpenKeyExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegCloseKey RegOpenKeyExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegCloseKey LdrGetProcedureAddress NtClose RegOpenKeyExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegCloseKey RegOpenKeyExW LdrLoadDll LdrGetProcedureAddress RegEnumKeyW RegOpenKeyExW RegQueryValueExW RegCloseKey RegEnumKeyW RegCloseKey LdrGetProcedureAddress RegOpenKeyExW RegOpenKeyExW NtCreateFile NtClose NtQueryDirectoryFile NtClose LdrGetProcedureAddress CoCreateInstance NtOpenSection NtOpenSection CreateDirectoryW NtCreateFile GetSystemWindowsDirectoryW GetSystemWindowsDirectoryW GetSystemWindowsDirectoryW LoadStringW GetSystemWindowsDirectoryW GetSystemDirectoryW RegOpenKeyExW LdrLoadDll LdrGetProcedureAddress RegQueryValueExW RegCloseKey RegOpenKeyExW RegQueryValueExW RegCloseKey NtCreateMutant NtCreateMutant GetNativeSystemInfo GetSystemWindowsDirectoryW GetSystemWindowsDirectoryW NtClose LdrLoadDll LdrGetProcedureAddress LdrLoadDll NtQuerySystemInformation RegOpenKeyExA RegQueryValueExA RegCloseKey NtOpenKey NtQueryValueKey NtClose NtOpenKey NtQueryValueKey NtClose NtOpenKey NtQueryValueKey NtClose RegOpenKeyExW GlobalMemoryStatusEx NtOpenKey NtOpenKey NtQueryValueKey NtClose NtDuplicateObject LdrGetProcedureAddress NtDuplicateObject NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory GetVolumeNameForVolumeMountPointW NtClose RegOpenKeyExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegCloseKey RegOpenKeyExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegCloseKey NtClose LdrGetProcedureAddress LdrGetProcedureAddress RegOpenKeyExW RegQueryValueExW RegQueryValueExW GetSystemTimeAsFileTime GetSystemTimeAsFileTime RegOpenKeyExW RegQueryValueExW RegCloseKey RegOpenKeyExW RegQueryValueExW RegCloseKey RegOpenKeyExW RegQueryValueExW RegCloseKey LdrLoadDll LdrGetProcedureAddress RegCloseKey NtClose LdrGetProcedureAddress NtCreateSection NtClose NtMapViewOfSection NtDuplicateObject GetVolumeNameForVolumeMountPointW NtClose RegOpenKeyExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegCloseKey RegOpenKeyExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegCloseKey NtDuplicateObject NtClose GetVolumeNameForVolumeMountPointW NtClose RegOpenKeyExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegCloseKey RegOpenKeyExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegCloseKey LdrGetProcedureAddress GetVolumePathNamesForVolumeNameW GetVolumePathNamesForVolumeNameW NtClose GetVolumePathNamesForVolumeNameW GetVolumePathNamesForVolumeNameW NtClose GetVolumePathNamesForVolumeNameW GetVolumePathNamesForVolumeNameW GetVolumePathNamesForVolumeNameW GetVolumePathNamesForVolumeNameW NtClose LdrGetProcedureAddress LdrUnloadDll NtClose NtOpenSection NtCreateFile NtClose NtCreateSection NtClose NtMapViewOfSection LdrGetProcedureAddress LdrGetProcedureAddress GetSystemTimeAsFileTime NtOpenSection NtMapViewOfSection GetSystemTimeAsFileTime GetSystemTimeAsFileTime GetSystemTimeAsFileTime NtClose NtClose NtUnmapViewOfSection NtCreateFile GetFileSizeEx NtReadFile GetFileInformationByHandleEx NtClose GetSystemTimeAsFileTime LdrGetProcedureAddress GetSystemTimeAsFileTime RegOpenKeyExW RegQueryValueExW RegCloseKey RegOpenKeyExW LdrLoadDll LdrGetProcedureAddress RegOpenKeyExW RegOpenKeyExW RegQueryValueExW RegQueryValueExW RegCloseKey RegOpenKeyExW RegQueryValueExW RegCloseKey RegOpenKeyExW RegOpenKeyExW RegQueryValueExW RegCloseKey RegOpenKeyExW RegOpenKeyExW RegQueryValueExW RegCloseKey RegOpenKeyExW RegOpenKeyExW RegQueryValueExW RegCloseKey RegOpenKeyExW RegOpenKeyExW RegQueryValueExW RegCloseKey RegOpenKeyExW RegOpenKeyExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegCloseKey LdrLoadDll LdrGetProcedureAddress RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegCloseKey RegOpenKeyExW RegCloseKey RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegQueryValueExW RegOpenKeyExW RegQueryValueExW RegOpenKeyExW RegQueryValueExW RegOpenKeyExW RegQueryValueExW RegOpenKeyExW RegQueryValueExW RegOpenKeyExW RegQueryValueExW RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegCloseKey RegCloseKey RegCloseKey NtCreateFile NtClose NtQueryDirectoryFile NtClose GetSystemTimeAsFileTime NtCreateFile NtClose NtQueryDirectoryFile NtClose NtCreateFile NtClose NtQueryDirectoryFile NtClose NtCreateFile NtClose NtQueryDirectoryFile NtClose RegOpenKeyExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegOpenKeyExW RegCloseKey LdrGetProcedureAddress CoInitializeEx NtOpenProcess NtClose RegOpenKeyExW RegOpenKeyExW RegCloseKey NtClose NtOpenKey RegOpenKeyExW RegCloseKey RegQueryValueExW RegCloseKey GetSystemTimeAsFileTime GetFileAttributesExW NtOpenFile NtQueryInformationFile NtAllocateVirtualMemory NtAllocateVirtualMemory NtReadFile NtFreeVirtualMemory NtClose NtOpenFile NtQueryInformationFile NtAllocateVirtualMemory NtAllocateVirtualMemory NtReadFile NtFreeVirtualMemory NtClose NtOpenFile NtQueryInformationFile NtAllocateVirtualMemory NtAllocateVirtualMemory NtReadFile NtFreeVirtualMemory NtClose LdrGetProcedureAddress CoUninitialize RegOpenKeyExW RegOpenKeyExW GetSystemTimeAsFileTime RegOpenKeyExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegOpenKeyExW RegCloseKey CoInitializeEx NtOpenProcess NtClose RegOpenKeyExW RegOpenKeyExW RegCloseKey NtClose NtOpenKey RegOpenKeyExW RegCloseKey RegQueryValueExW RegOpenKeyExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegOpenKeyExW RegCloseKey NtOpenProcess NtClose RegOpenKeyExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegCloseKey CoUninitialize GetSystemTimeAsFileTime RegOpenKeyExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegOpenKeyExW RegCloseKey CoInitializeEx LdrLoadDll LdrGetProcedureAddress LdrLoadDll LdrGetProcedureAddress RegOpenKeyExW RegQueryValueExW RegQueryValueExW RegCloseKey NtClose CoUninitialize GetSystemTimeAsFileTime RegOpenKeyExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegOpenKeyExW RegCloseKey CoInitializeEx CoUninitialize GetSystemTimeAsFileTime RegOpenKeyExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegCloseKey RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegOpenKeyExW RegQueryValueExW RegCloseKey LdrGetDllHandle LdrGetDllHandle LdrGetProcedureAddress LdrGetProcedureAddress RegOpenKeyExW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegEnumKeyW RegCloseKey RegOpenKeyExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegOpenKeyExW RegCloseKey NtOpenProcess NtClose RegOpenKeyExW RegOpenKeyExW RegCloseKey NtClose NtOpenKey RegOpenKeyExW RegCloseKey RegQueryValueExW RegOpenKeyExW RegQueryValueExW RegQueryValueExW RegCloseKey NtClose RegCloseKey RegOpenKeyExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegOpenKeyExW RegCloseKey RegOpenKeyExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegOpenKeyExW RegCloseKey RegOpenKeyExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegOpenKeyExW RegCloseKey RegOpenKeyExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegOpenKeyExW RegCloseKey RegOpenKeyExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegOpenKeyExW RegCloseKey RegOpenKeyExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegOpenKeyExW RegCloseKey RegOpenKeyExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegOpenKeyExW RegCloseKey RegOpenKeyExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegOpenKeyExW RegCloseKey RegOpenKeyExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegOpenKeyExW RegCloseKey RegOpenKeyExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegOpenKeyExW RegCloseKey NtOpenProcess NtClose RegOpenKeyExW RegOpenKeyExW RegCloseKey NtClose NtOpenKey RegOpenKeyExW RegCloseKey RegQueryValueExW RegCloseKey RegOpenKeyExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegOpenKeyExW RegCloseKey RegOpenKeyExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegOpenKeyExW RegCloseKey RegOpenKeyExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegOpenKeyExW RegCloseKey RegOpenKeyExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegOpenKeyExW RegCloseKey RegOpenKeyExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegOpenKeyExW RegCloseKey RegOpenKeyExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegOpenKeyExW RegCloseKey RegOpenKeyExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegOpenKeyExW RegCloseKey NtOpenProcess NtClose RegOpenKeyExW RegOpenKeyExW RegCloseKey NtClose NtOpenKey RegOpenKeyExW RegCloseKey RegQueryValueExW RegCloseKey RegOpenKeyExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegOpenKeyExW RegCloseKey RegOpenKeyExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegOpenKeyExW RegCloseKey RegOpenKeyExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegOpenKeyExW RegCloseKey RegOpenKeyExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegOpenKeyExW RegCloseKey NtFreeVirtualMemory NtFreeVirtualMemory RegOpenKeyExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW NtAllocateVirtualMemory RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegOpenKeyExW RegCloseKey RegOpenKeyExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegOpenKeyExW RegCloseKey RegOpenKeyExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegOpenKeyExW RegCloseKey RegOpenKeyExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegOpenKeyExW RegCloseKey RegOpenKeyExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegOpenKeyExW RegCloseKey RegOpenKeyExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegOpenKeyExW RegCloseKey RegOpenKeyExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegOpenKeyExW RegCloseKey RegOpenKeyExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegOpenKeyExW RegCloseKey RegOpenKeyExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegOpenKeyExW RegCloseKey RegOpenKeyExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegOpenKeyExW RegCloseKey RegOpenKeyExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegOpenKeyExW RegCloseKey NtOpenProcess NtClose RegOpenKeyExW RegOpenKeyExW RegCloseKey NtClose NtOpenKey RegOpenKeyExW RegCloseKey RegQueryValueExW RegOpenKeyExW RegQueryValueExW RegQueryValueExW RegCloseKey NtClose RegCloseKey RegOpenKeyExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegOpenKeyExW RegCloseKey RegOpenKeyExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegOpenKeyExW RegCloseKey RegOpenKeyExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegOpenKeyExW RegCloseKey RegOpenKeyExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegOpenKeyExW RegCloseKey RegOpenKeyExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegOpenKeyExW RegCloseKey RegOpenKeyExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegOpenKeyExW RegCloseKey RegOpenKeyExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegOpenKeyExW RegCloseKey RegOpenKeyExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegOpenKeyExW RegCloseKey NtOpenProcess NtClose RegOpenKeyExW RegOpenKeyExW RegCloseKey NtClose NtOpenKey RegOpenKeyExW RegCloseKey RegQueryValueExW RegCloseKey RegOpenKeyExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegOpenKeyExW RegCloseKey RegOpenKeyExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegOpenKeyExW RegCloseKey RegOpenKeyExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegOpenKeyExW RegCloseKey RegOpenKeyExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegOpenKeyExW RegCloseKey RegOpenKeyExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegOpenKeyExW RegCloseKey RegOpenKeyExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegOpenKeyExW RegCloseKey NtOpenProcess NtClose RegOpenKeyExW RegOpenKeyExW RegCloseKey NtClose NtOpenKey RegOpenKeyExW RegCloseKey RegQueryValueExW RegCloseKey RegOpenKeyExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegOpenKeyExW RegCloseKey RegOpenKeyExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegOpenKeyExW RegCloseKey RegOpenKeyExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegOpenKeyExW RegCloseKey RegOpenKeyExW RegOpenKeyExW RegCloseKey RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQueryValueExW RegQue</t>
+  </si>
+  <si>
+    <t>192.168.56.101:49360 192.168.56.101:64412 192.168.56.101:58084 192.168.56.101:54425 192.168.56.101:52057 192.168.56.101:59469 192.168.56.101:54227 192.168.56.101:52887 192.168.56.101:50300 192.168.56.101:137 192.168.56.101:1900 192.168.56.101:52889 192.168.56.101:63529 192.168.56.101:63530 192.168.56.101:51765 192.168.56.101:138 192.168.56.101:49465 192.168.56.101:50974 192.168.56.101:55167 192.168.56.101:63794 192.168.56.101:62948 192.168.56.101:49746 192.168.56.101:53485 192.168.56.101:54813 192.168.56.101:63393 192.168.56.101:61926 192.168.56.101:55972 192.168.56.101:50766 192.168.56.101:51753 192.168.56.101:50018 192.168.56.101:50988 192.168.56.101:62982 192.168.56.101:56409 192.168.56.101:60009 192.168.56.101:50639 192.168.56.101:53003 192.168.56.101:58359 192.168.56.101:61815 192.168.56.101:64235 192.168.56.101:52402 192.168.56.101:62413 192.168.56.101:59538 192.168.56.101:64855</t>
+  </si>
+  <si>
+    <t>224.0.0.252:5355 224.0.0.252:5355 224.0.0.252:5355 224.0.0.252:5355 224.0.0.252:5355 224.0.0.252:5355 224.0.0.252:5355 8.8.8.8:53 239.255.255.250:3702 192.168.56.255:137 239.255.255.250:1900 239.255.255.250:1900 224.0.0.252:5355 239.255.255.250:3702 224.0.0.252:5355 192.168.56.255:138 8.8.8.8:53 224.0.0.252:5355 8.8.8.8:53 8.8.8.8:53 224.0.0.252:5355 224.0.0.252:5355 224.0.0.252:5355 224.0.0.252:5355 8.8.8.8:53 8.8.8.8:53 224.0.0.252:5355 224.0.0.252:5355 224.0.0.252:5355 224.0.0.252:5355 8.8.8.8:53 8.8.8.8:53 224.0.0.252:5355 224.0.0.252:5355 224.0.0.252:5355 224.0.0.252:5355 224.0.0.252:5355 224.0.0.252:5355 8.8.8.8:53 8.8.8.8:53 8.8.8.8:53 8.8.8.8:53 8.8.8.8:53</t>
   </si>
 </sst>
 </file>

</xml_diff>